<commit_message>
Some KlebSeq assays need multiple lines
</commit_message>
<xml_diff>
--- a/assay_data/KlebSeq_assays.xlsx
+++ b/assay_data/KlebSeq_assays.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19720" windowHeight="22900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="36560" windowHeight="23020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Assays" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="459">
   <si>
     <t>Assay Name</t>
   </si>
@@ -2095,6 +2095,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2107,7 +2108,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="331">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -2769,10 +2769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE175"/>
+  <dimension ref="A1:AE188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="A138" sqref="A138:XFD138"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="M153" sqref="M153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2797,31 +2797,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="1" customFormat="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="21" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21" t="s">
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
       <c r="P1" s="3" t="s">
         <v>19</v>
       </c>
@@ -4156,7 +4156,7 @@
       <c r="C63" t="s">
         <v>23</v>
       </c>
-      <c r="D63" s="25" t="s">
+      <c r="D63" s="21" t="s">
         <v>184</v>
       </c>
       <c r="I63" t="s">
@@ -4176,7 +4176,7 @@
       <c r="C64" t="s">
         <v>28</v>
       </c>
-      <c r="D64" s="25" t="s">
+      <c r="D64" s="21" t="s">
         <v>188</v>
       </c>
       <c r="I64" s="9" t="s">
@@ -4196,7 +4196,7 @@
       <c r="C65" t="s">
         <v>28</v>
       </c>
-      <c r="D65" s="25" t="s">
+      <c r="D65" s="21" t="s">
         <v>192</v>
       </c>
       <c r="I65" s="9" t="s">
@@ -4216,7 +4216,7 @@
       <c r="C66" t="s">
         <v>28</v>
       </c>
-      <c r="D66" s="25" t="s">
+      <c r="D66" s="21" t="s">
         <v>195</v>
       </c>
       <c r="I66" s="9" t="s">
@@ -4236,7 +4236,7 @@
       <c r="C67" t="s">
         <v>28</v>
       </c>
-      <c r="D67" s="25" t="s">
+      <c r="D67" s="21" t="s">
         <v>198</v>
       </c>
       <c r="I67" s="9" t="s">
@@ -4256,7 +4256,7 @@
       <c r="C68" t="s">
         <v>28</v>
       </c>
-      <c r="D68" s="25" t="s">
+      <c r="D68" s="21" t="s">
         <v>201</v>
       </c>
       <c r="I68" s="9" t="s">
@@ -4276,7 +4276,7 @@
       <c r="C69" t="s">
         <v>28</v>
       </c>
-      <c r="D69" s="25" t="s">
+      <c r="D69" s="21" t="s">
         <v>205</v>
       </c>
       <c r="I69" s="9" t="s">
@@ -4296,7 +4296,7 @@
       <c r="C70" t="s">
         <v>28</v>
       </c>
-      <c r="D70" s="25" t="s">
+      <c r="D70" s="21" t="s">
         <v>209</v>
       </c>
       <c r="I70" s="9" t="s">
@@ -4316,7 +4316,7 @@
       <c r="C71" t="s">
         <v>28</v>
       </c>
-      <c r="D71" s="25" t="s">
+      <c r="D71" s="21" t="s">
         <v>212</v>
       </c>
       <c r="I71" s="9" t="s">
@@ -4336,7 +4336,7 @@
       <c r="C72" t="s">
         <v>28</v>
       </c>
-      <c r="D72" s="25" t="s">
+      <c r="D72" s="21" t="s">
         <v>215</v>
       </c>
       <c r="I72" s="9" t="s">
@@ -4356,7 +4356,7 @@
       <c r="C73" t="s">
         <v>28</v>
       </c>
-      <c r="D73" s="25" t="s">
+      <c r="D73" s="21" t="s">
         <v>218</v>
       </c>
       <c r="I73" s="9" t="s">
@@ -4376,7 +4376,7 @@
       <c r="C74" t="s">
         <v>28</v>
       </c>
-      <c r="D74" s="25" t="s">
+      <c r="D74" s="21" t="s">
         <v>222</v>
       </c>
       <c r="I74" s="9" t="s">
@@ -4396,7 +4396,7 @@
       <c r="C75" t="s">
         <v>28</v>
       </c>
-      <c r="D75" s="25" t="s">
+      <c r="D75" s="21" t="s">
         <v>225</v>
       </c>
       <c r="I75" s="9" t="s">
@@ -4416,7 +4416,7 @@
       <c r="C76" t="s">
         <v>28</v>
       </c>
-      <c r="D76" s="25" t="s">
+      <c r="D76" s="21" t="s">
         <v>229</v>
       </c>
       <c r="I76" s="9" t="s">
@@ -4436,7 +4436,7 @@
       <c r="C77" t="s">
         <v>28</v>
       </c>
-      <c r="D77" s="25" t="s">
+      <c r="D77" s="21" t="s">
         <v>233</v>
       </c>
       <c r="I77" s="9" t="s">
@@ -4456,7 +4456,7 @@
       <c r="C78" t="s">
         <v>26</v>
       </c>
-      <c r="D78" s="25" t="s">
+      <c r="D78" s="21" t="s">
         <v>237</v>
       </c>
       <c r="I78" s="9" t="s">
@@ -4476,7 +4476,7 @@
       <c r="C79" t="s">
         <v>26</v>
       </c>
-      <c r="D79" s="25" t="s">
+      <c r="D79" s="21" t="s">
         <v>237</v>
       </c>
       <c r="I79" s="9" t="s">
@@ -4502,7 +4502,7 @@
       <c r="C80" t="s">
         <v>26</v>
       </c>
-      <c r="D80" s="25" t="s">
+      <c r="D80" s="21" t="s">
         <v>244</v>
       </c>
       <c r="I80" s="9" t="s">
@@ -4522,7 +4522,7 @@
       <c r="C81" t="s">
         <v>26</v>
       </c>
-      <c r="D81" s="25" t="s">
+      <c r="D81" s="21" t="s">
         <v>248</v>
       </c>
       <c r="I81" s="9" t="s">
@@ -4542,7 +4542,7 @@
       <c r="C82" t="s">
         <v>26</v>
       </c>
-      <c r="D82" s="25" t="s">
+      <c r="D82" s="21" t="s">
         <v>248</v>
       </c>
       <c r="I82" s="9" t="s">
@@ -4562,7 +4562,7 @@
       <c r="C83" t="s">
         <v>26</v>
       </c>
-      <c r="D83" s="25" t="s">
+      <c r="D83" s="21" t="s">
         <v>255</v>
       </c>
       <c r="I83" s="9" t="s">
@@ -4582,7 +4582,7 @@
       <c r="C84" t="s">
         <v>26</v>
       </c>
-      <c r="D84" s="25" t="s">
+      <c r="D84" s="21" t="s">
         <v>248</v>
       </c>
       <c r="I84" s="9" t="s">
@@ -4602,7 +4602,7 @@
       <c r="C85" t="s">
         <v>26</v>
       </c>
-      <c r="D85" s="25" t="s">
+      <c r="D85" s="21" t="s">
         <v>261</v>
       </c>
       <c r="I85" s="9" t="s">
@@ -4622,7 +4622,7 @@
       <c r="C86" t="s">
         <v>26</v>
       </c>
-      <c r="D86" s="25" t="s">
+      <c r="D86" s="21" t="s">
         <v>265</v>
       </c>
       <c r="I86" s="9" t="s">
@@ -4642,7 +4642,7 @@
       <c r="C87" t="s">
         <v>26</v>
       </c>
-      <c r="D87" s="25" t="s">
+      <c r="D87" s="21" t="s">
         <v>268</v>
       </c>
       <c r="I87" s="9" t="s">
@@ -4662,7 +4662,7 @@
       <c r="C88" t="s">
         <v>26</v>
       </c>
-      <c r="D88" s="25" t="s">
+      <c r="D88" s="21" t="s">
         <v>271</v>
       </c>
       <c r="I88" s="9" t="s">
@@ -4682,7 +4682,7 @@
       <c r="C89" t="s">
         <v>26</v>
       </c>
-      <c r="D89" s="25" t="s">
+      <c r="D89" s="21" t="s">
         <v>275</v>
       </c>
       <c r="I89" s="9" t="s">
@@ -4702,7 +4702,7 @@
       <c r="C90" t="s">
         <v>26</v>
       </c>
-      <c r="D90" s="25" t="s">
+      <c r="D90" s="21" t="s">
         <v>279</v>
       </c>
       <c r="I90" s="9" t="s">
@@ -4722,7 +4722,7 @@
       <c r="C91" t="s">
         <v>26</v>
       </c>
-      <c r="D91" s="25" t="s">
+      <c r="D91" s="21" t="s">
         <v>282</v>
       </c>
       <c r="I91" s="9" t="s">
@@ -4742,7 +4742,7 @@
       <c r="C92" t="s">
         <v>26</v>
       </c>
-      <c r="D92" s="25" t="s">
+      <c r="D92" s="21" t="s">
         <v>286</v>
       </c>
       <c r="I92" s="9" t="s">
@@ -4762,7 +4762,7 @@
       <c r="C93" t="s">
         <v>26</v>
       </c>
-      <c r="D93" s="25" t="s">
+      <c r="D93" s="21" t="s">
         <v>290</v>
       </c>
       <c r="I93" s="9" t="s">
@@ -4782,7 +4782,7 @@
       <c r="C94" t="s">
         <v>26</v>
       </c>
-      <c r="D94" s="25" t="s">
+      <c r="D94" s="21" t="s">
         <v>293</v>
       </c>
       <c r="I94" s="9" t="s">
@@ -4802,7 +4802,7 @@
       <c r="C95" t="s">
         <v>26</v>
       </c>
-      <c r="D95" s="25" t="s">
+      <c r="D95" s="21" t="s">
         <v>296</v>
       </c>
       <c r="I95" s="9" t="s">
@@ -4822,7 +4822,7 @@
       <c r="C96" t="s">
         <v>23</v>
       </c>
-      <c r="D96" s="25" t="s">
+      <c r="D96" s="21" t="s">
         <v>299</v>
       </c>
       <c r="I96" s="9" t="s">
@@ -4851,7 +4851,7 @@
       <c r="C97" t="s">
         <v>23</v>
       </c>
-      <c r="D97" s="25" t="s">
+      <c r="D97" s="21" t="s">
         <v>303</v>
       </c>
       <c r="I97" s="9" t="s">
@@ -4880,7 +4880,7 @@
       <c r="C98" t="s">
         <v>23</v>
       </c>
-      <c r="D98" s="25" t="s">
+      <c r="D98" s="21" t="s">
         <v>307</v>
       </c>
       <c r="I98" s="9" t="s">
@@ -4909,7 +4909,7 @@
       <c r="C99" t="s">
         <v>23</v>
       </c>
-      <c r="D99" s="25" t="s">
+      <c r="D99" s="21" t="s">
         <v>312</v>
       </c>
       <c r="I99" s="9" t="s">
@@ -4938,7 +4938,7 @@
       <c r="C100" t="s">
         <v>23</v>
       </c>
-      <c r="D100" s="25" t="s">
+      <c r="D100" s="21" t="s">
         <v>316</v>
       </c>
       <c r="I100" s="9" t="s">
@@ -4967,7 +4967,7 @@
       <c r="C101" t="s">
         <v>23</v>
       </c>
-      <c r="D101" s="25" t="s">
+      <c r="D101" s="21" t="s">
         <v>321</v>
       </c>
       <c r="I101" s="9" t="s">
@@ -4996,7 +4996,7 @@
       <c r="C102" t="s">
         <v>23</v>
       </c>
-      <c r="D102" s="25" t="s">
+      <c r="D102" s="21" t="s">
         <v>321</v>
       </c>
       <c r="I102" s="9" t="s">
@@ -5025,7 +5025,7 @@
       <c r="C103" t="s">
         <v>23</v>
       </c>
-      <c r="D103" s="25" t="s">
+      <c r="D103" s="21" t="s">
         <v>328</v>
       </c>
       <c r="I103" s="9" t="s">
@@ -5054,7 +5054,7 @@
       <c r="C104" t="s">
         <v>23</v>
       </c>
-      <c r="D104" s="25" t="s">
+      <c r="D104" s="21" t="s">
         <v>332</v>
       </c>
       <c r="I104" s="9" t="s">
@@ -5083,7 +5083,7 @@
       <c r="C105" t="s">
         <v>23</v>
       </c>
-      <c r="D105" s="25" t="s">
+      <c r="D105" s="21" t="s">
         <v>336</v>
       </c>
       <c r="I105" s="9" t="s">
@@ -5112,7 +5112,7 @@
       <c r="C106" t="s">
         <v>23</v>
       </c>
-      <c r="D106" s="25" t="s">
+      <c r="D106" s="21" t="s">
         <v>340</v>
       </c>
       <c r="I106" s="9" t="s">
@@ -5141,7 +5141,7 @@
       <c r="C107" t="s">
         <v>23</v>
       </c>
-      <c r="D107" s="25" t="s">
+      <c r="D107" s="21" t="s">
         <v>344</v>
       </c>
       <c r="I107" s="9" t="s">
@@ -5170,7 +5170,7 @@
       <c r="C108" t="s">
         <v>23</v>
       </c>
-      <c r="D108" s="25" t="s">
+      <c r="D108" s="21" t="s">
         <v>348</v>
       </c>
       <c r="I108" s="9" t="s">
@@ -5199,7 +5199,7 @@
       <c r="C109" t="s">
         <v>23</v>
       </c>
-      <c r="D109" s="25" t="s">
+      <c r="D109" s="21" t="s">
         <v>352</v>
       </c>
       <c r="I109" s="9" t="s">
@@ -5228,7 +5228,7 @@
       <c r="C110" t="s">
         <v>23</v>
       </c>
-      <c r="D110" s="25" t="s">
+      <c r="D110" s="21" t="s">
         <v>356</v>
       </c>
       <c r="I110" s="9" t="s">
@@ -5257,7 +5257,7 @@
       <c r="C111" t="s">
         <v>23</v>
       </c>
-      <c r="D111" s="25" t="s">
+      <c r="D111" s="21" t="s">
         <v>360</v>
       </c>
       <c r="I111" s="9" t="s">
@@ -5286,7 +5286,7 @@
       <c r="C112" t="s">
         <v>23</v>
       </c>
-      <c r="D112" s="25" t="s">
+      <c r="D112" s="21" t="s">
         <v>364</v>
       </c>
       <c r="I112" s="9" t="s">
@@ -5315,7 +5315,7 @@
       <c r="C113" t="s">
         <v>23</v>
       </c>
-      <c r="D113" s="25" t="s">
+      <c r="D113" s="21" t="s">
         <v>368</v>
       </c>
       <c r="I113" s="9" t="s">
@@ -5344,7 +5344,7 @@
       <c r="C114" t="s">
         <v>23</v>
       </c>
-      <c r="D114" s="25" t="s">
+      <c r="D114" s="21" t="s">
         <v>372</v>
       </c>
       <c r="I114" s="9" t="s">
@@ -5373,7 +5373,7 @@
       <c r="C115" t="s">
         <v>23</v>
       </c>
-      <c r="D115" s="25" t="s">
+      <c r="D115" s="21" t="s">
         <v>376</v>
       </c>
       <c r="I115" s="9" t="s">
@@ -5409,7 +5409,7 @@
       <c r="C117" t="s">
         <v>23</v>
       </c>
-      <c r="D117" s="25" t="s">
+      <c r="D117" s="21" t="s">
         <v>380</v>
       </c>
       <c r="I117" s="9" t="s">
@@ -5438,7 +5438,7 @@
       <c r="C118" t="s">
         <v>23</v>
       </c>
-      <c r="D118" s="25" t="s">
+      <c r="D118" s="21" t="s">
         <v>384</v>
       </c>
       <c r="I118" s="9" t="s">
@@ -5467,7 +5467,7 @@
       <c r="C119" t="s">
         <v>23</v>
       </c>
-      <c r="D119" s="25" t="s">
+      <c r="D119" s="21" t="s">
         <v>389</v>
       </c>
       <c r="I119" s="9" t="s">
@@ -5496,7 +5496,7 @@
       <c r="C120" t="s">
         <v>23</v>
       </c>
-      <c r="D120" s="25" t="s">
+      <c r="D120" s="21" t="s">
         <v>393</v>
       </c>
       <c r="I120" s="9" t="s">
@@ -5525,7 +5525,7 @@
       <c r="C121" t="s">
         <v>23</v>
       </c>
-      <c r="D121" s="25"/>
+      <c r="D121" s="21"/>
       <c r="I121" s="9" t="s">
         <v>397</v>
       </c>
@@ -5552,7 +5552,7 @@
       <c r="C122" t="s">
         <v>23</v>
       </c>
-      <c r="D122" s="25" t="s">
+      <c r="D122" s="21" t="s">
         <v>399</v>
       </c>
       <c r="I122" s="9" t="s">
@@ -5581,7 +5581,7 @@
       <c r="C123" t="s">
         <v>23</v>
       </c>
-      <c r="D123" s="25"/>
+      <c r="D123" s="21"/>
       <c r="I123" s="9" t="s">
         <v>403</v>
       </c>
@@ -5635,7 +5635,7 @@
       <c r="C125" t="s">
         <v>23</v>
       </c>
-      <c r="D125" s="25" t="s">
+      <c r="D125" s="21" t="s">
         <v>409</v>
       </c>
       <c r="I125" s="9" t="s">
@@ -5664,7 +5664,7 @@
       <c r="C126" t="s">
         <v>23</v>
       </c>
-      <c r="D126" s="25"/>
+      <c r="D126" s="21"/>
       <c r="I126" s="9" t="s">
         <v>413</v>
       </c>
@@ -5691,7 +5691,7 @@
       <c r="C127" t="s">
         <v>23</v>
       </c>
-      <c r="D127" s="25" t="s">
+      <c r="D127" s="21" t="s">
         <v>416</v>
       </c>
       <c r="I127" s="9" t="s">
@@ -5720,7 +5720,7 @@
       <c r="C128" t="s">
         <v>23</v>
       </c>
-      <c r="D128" s="25" t="s">
+      <c r="D128" s="21" t="s">
         <v>419</v>
       </c>
       <c r="I128" s="9" t="s">
@@ -5749,7 +5749,7 @@
       <c r="C129" t="s">
         <v>23</v>
       </c>
-      <c r="D129" s="25" t="s">
+      <c r="D129" s="21" t="s">
         <v>422</v>
       </c>
       <c r="I129" s="9" t="s">
@@ -5778,7 +5778,7 @@
       <c r="C130" t="s">
         <v>23</v>
       </c>
-      <c r="D130" s="25" t="s">
+      <c r="D130" s="21" t="s">
         <v>426</v>
       </c>
       <c r="I130" s="9" t="s">
@@ -5807,7 +5807,7 @@
       <c r="C131" t="s">
         <v>23</v>
       </c>
-      <c r="D131" s="25"/>
+      <c r="D131" s="21"/>
       <c r="I131" s="9" t="s">
         <v>430</v>
       </c>
@@ -5834,7 +5834,7 @@
       <c r="C132" t="s">
         <v>23</v>
       </c>
-      <c r="D132" s="25" t="s">
+      <c r="D132" s="21" t="s">
         <v>433</v>
       </c>
       <c r="I132" s="9" t="s">
@@ -5863,7 +5863,7 @@
       <c r="C133" t="s">
         <v>22</v>
       </c>
-      <c r="D133" s="25" t="s">
+      <c r="D133" s="21" t="s">
         <v>437</v>
       </c>
       <c r="I133" s="9" t="s">
@@ -5883,264 +5883,472 @@
       </c>
     </row>
     <row r="134" spans="1:16">
-      <c r="A134" t="s">
+      <c r="D134" s="21"/>
+      <c r="I134" s="9"/>
+      <c r="J134">
+        <v>67</v>
+      </c>
+      <c r="K134" t="s">
+        <v>181</v>
+      </c>
+      <c r="L134" t="s">
+        <v>180</v>
+      </c>
+      <c r="P134" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16">
+      <c r="D135" s="21"/>
+      <c r="I135" s="9"/>
+      <c r="J135">
+        <v>91</v>
+      </c>
+      <c r="K135" t="s">
+        <v>180</v>
+      </c>
+      <c r="L135" t="s">
+        <v>181</v>
+      </c>
+      <c r="P135" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16">
+      <c r="D136" s="21"/>
+      <c r="I136" s="9"/>
+      <c r="J136">
+        <v>126</v>
+      </c>
+      <c r="K136" t="s">
+        <v>309</v>
+      </c>
+      <c r="L136" t="s">
+        <v>318</v>
+      </c>
+      <c r="P136" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16">
+      <c r="D137" s="21"/>
+      <c r="I137" s="9"/>
+      <c r="J137">
+        <v>143</v>
+      </c>
+      <c r="K137" t="s">
+        <v>309</v>
+      </c>
+      <c r="L137" t="s">
+        <v>181</v>
+      </c>
+      <c r="P137" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16">
+      <c r="D138" s="21"/>
+      <c r="I138" s="9"/>
+      <c r="J138">
+        <v>181</v>
+      </c>
+      <c r="K138" t="s">
+        <v>181</v>
+      </c>
+      <c r="L138" t="s">
+        <v>180</v>
+      </c>
+      <c r="P138" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16">
+      <c r="D139" s="21"/>
+      <c r="I139" s="9"/>
+      <c r="J139">
+        <v>184</v>
+      </c>
+      <c r="K139" t="s">
+        <v>309</v>
+      </c>
+      <c r="L139" t="s">
+        <v>181</v>
+      </c>
+      <c r="P139" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16">
+      <c r="D140" s="21"/>
+      <c r="I140" s="9"/>
+      <c r="J140">
+        <v>220</v>
+      </c>
+      <c r="K140" t="s">
+        <v>318</v>
+      </c>
+      <c r="L140" t="s">
+        <v>309</v>
+      </c>
+      <c r="P140" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16">
+      <c r="D141" s="21"/>
+      <c r="I141" s="9"/>
+      <c r="J141">
+        <v>235</v>
+      </c>
+      <c r="K141" t="s">
+        <v>318</v>
+      </c>
+      <c r="L141" t="s">
+        <v>309</v>
+      </c>
+      <c r="P141" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16">
+      <c r="A142" t="s">
         <v>440</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B142" t="s">
         <v>21</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C142" t="s">
         <v>22</v>
       </c>
-      <c r="D134" s="25"/>
-      <c r="I134" s="9" t="s">
+      <c r="D142" s="21"/>
+      <c r="I142" s="9" t="s">
         <v>441</v>
       </c>
-      <c r="J134">
+      <c r="J142">
         <v>39</v>
       </c>
-      <c r="K134" t="s">
+      <c r="K142" t="s">
         <v>318</v>
       </c>
-      <c r="L134" t="s">
+      <c r="L142" t="s">
         <v>309</v>
       </c>
-      <c r="P134" t="s">
+      <c r="P142" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="135" spans="1:16">
-      <c r="A135" t="s">
+    <row r="143" spans="1:16">
+      <c r="D143" s="21"/>
+      <c r="I143" s="9"/>
+      <c r="J143">
+        <v>51</v>
+      </c>
+      <c r="K143" t="s">
+        <v>318</v>
+      </c>
+      <c r="L143" t="s">
+        <v>309</v>
+      </c>
+      <c r="P143" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16">
+      <c r="D144" s="21"/>
+      <c r="I144" s="9"/>
+      <c r="J144">
+        <v>63</v>
+      </c>
+      <c r="K144" t="s">
+        <v>309</v>
+      </c>
+      <c r="L144" t="s">
+        <v>318</v>
+      </c>
+      <c r="P144" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16">
+      <c r="D145" s="21"/>
+      <c r="I145" s="9"/>
+      <c r="J145">
+        <v>78</v>
+      </c>
+      <c r="K145" t="s">
+        <v>318</v>
+      </c>
+      <c r="L145" t="s">
+        <v>180</v>
+      </c>
+      <c r="P145" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16">
+      <c r="D146" s="21"/>
+      <c r="I146" s="9"/>
+      <c r="J146">
+        <v>82</v>
+      </c>
+      <c r="K146" t="s">
+        <v>309</v>
+      </c>
+      <c r="L146" t="s">
+        <v>180</v>
+      </c>
+      <c r="P146" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16">
+      <c r="D147" s="21"/>
+      <c r="I147" s="9"/>
+      <c r="J147">
+        <v>147</v>
+      </c>
+      <c r="K147" t="s">
+        <v>181</v>
+      </c>
+      <c r="L147" t="s">
+        <v>180</v>
+      </c>
+      <c r="P147" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16">
+      <c r="A148" t="s">
         <v>443</v>
       </c>
-      <c r="B135" t="s">
-        <v>20</v>
-      </c>
-      <c r="C135" t="s">
-        <v>26</v>
-      </c>
-      <c r="D135" s="25" t="s">
+      <c r="B148" t="s">
+        <v>20</v>
+      </c>
+      <c r="C148" t="s">
+        <v>26</v>
+      </c>
+      <c r="D148" s="21" t="s">
         <v>444</v>
       </c>
-      <c r="I135" s="9" t="s">
+      <c r="I148" s="9" t="s">
         <v>445</v>
       </c>
-      <c r="P135" t="s">
+      <c r="P148" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="136" spans="1:16">
-      <c r="A136" t="s">
+    <row r="149" spans="1:16">
+      <c r="A149" t="s">
         <v>447</v>
       </c>
-      <c r="B136" t="s">
-        <v>20</v>
-      </c>
-      <c r="C136" t="s">
-        <v>26</v>
-      </c>
-      <c r="D136" s="25" t="s">
+      <c r="B149" t="s">
+        <v>20</v>
+      </c>
+      <c r="C149" t="s">
+        <v>26</v>
+      </c>
+      <c r="D149" s="21" t="s">
         <v>448</v>
       </c>
-      <c r="I136" s="9" t="s">
+      <c r="I149" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="P136" t="s">
+      <c r="P149" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="137" spans="1:16">
-      <c r="A137" t="s">
+    <row r="150" spans="1:16">
+      <c r="A150" t="s">
         <v>451</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B150" t="s">
         <v>25</v>
       </c>
-      <c r="C137" t="s">
-        <v>26</v>
-      </c>
-      <c r="D137" s="25" t="s">
+      <c r="C150" t="s">
+        <v>26</v>
+      </c>
+      <c r="D150" s="21" t="s">
         <v>452</v>
       </c>
-      <c r="I137" s="9" t="s">
+      <c r="I150" s="9" t="s">
         <v>453</v>
       </c>
-      <c r="P137" t="s">
+      <c r="P150" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="138" spans="1:16">
-      <c r="A138" t="s">
+    <row r="151" spans="1:16">
+      <c r="A151" t="s">
         <v>455</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B151" t="s">
         <v>25</v>
       </c>
-      <c r="C138" t="s">
-        <v>26</v>
-      </c>
-      <c r="D138" s="25" t="s">
+      <c r="C151" t="s">
+        <v>26</v>
+      </c>
+      <c r="D151" s="21" t="s">
         <v>456</v>
       </c>
-      <c r="I138" s="9" t="s">
+      <c r="I151" s="9" t="s">
         <v>457</v>
       </c>
-      <c r="P138" t="s">
+      <c r="P151" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="139" spans="1:16">
-      <c r="I139" s="9"/>
-      <c r="P139" s="12"/>
-    </row>
-    <row r="140" spans="1:16">
-      <c r="I140" s="9"/>
-      <c r="P140" s="12"/>
-    </row>
-    <row r="141" spans="1:16">
-      <c r="I141" s="9"/>
-      <c r="P141" s="12"/>
-    </row>
-    <row r="142" spans="1:16">
-      <c r="I142" s="9"/>
-      <c r="P142" s="12"/>
-    </row>
-    <row r="143" spans="1:16">
-      <c r="D143" s="9"/>
-      <c r="I143" s="9"/>
-    </row>
-    <row r="144" spans="1:16">
-      <c r="D144" s="9"/>
-      <c r="I144" s="9"/>
-    </row>
-    <row r="145" spans="4:18">
-      <c r="I145" s="9"/>
-      <c r="P145" s="15"/>
-    </row>
-    <row r="146" spans="4:18">
-      <c r="I146" s="9"/>
-      <c r="P146" s="15"/>
-    </row>
-    <row r="147" spans="4:18">
-      <c r="D147" s="9"/>
-      <c r="I147" s="9"/>
-    </row>
-    <row r="148" spans="4:18">
-      <c r="D148" s="9"/>
-      <c r="I148" s="9"/>
-    </row>
-    <row r="149" spans="4:18">
-      <c r="D149" s="9"/>
-      <c r="I149" s="9"/>
-    </row>
-    <row r="150" spans="4:18">
-      <c r="D150" s="9"/>
-      <c r="I150" s="9"/>
-    </row>
-    <row r="151" spans="4:18">
-      <c r="D151" s="9"/>
-      <c r="I151" s="9"/>
-    </row>
-    <row r="152" spans="4:18">
-      <c r="D152" s="9"/>
+    <row r="152" spans="1:16">
       <c r="I152" s="9"/>
-      <c r="R152" s="17"/>
-    </row>
-    <row r="153" spans="4:18">
-      <c r="D153" s="9"/>
+      <c r="P152" s="12"/>
+    </row>
+    <row r="153" spans="1:16">
       <c r="I153" s="9"/>
-    </row>
-    <row r="154" spans="4:18">
-      <c r="D154" s="9"/>
+      <c r="P153" s="12"/>
+    </row>
+    <row r="154" spans="1:16">
       <c r="I154" s="9"/>
-      <c r="P154" s="18"/>
-    </row>
-    <row r="155" spans="4:18">
+      <c r="P154" s="12"/>
+    </row>
+    <row r="155" spans="1:16">
       <c r="I155" s="9"/>
-    </row>
-    <row r="156" spans="4:18">
+      <c r="P155" s="12"/>
+    </row>
+    <row r="156" spans="1:16">
+      <c r="D156" s="9"/>
       <c r="I156" s="9"/>
     </row>
-    <row r="157" spans="4:18">
+    <row r="157" spans="1:16">
+      <c r="D157" s="9"/>
       <c r="I157" s="9"/>
     </row>
-    <row r="158" spans="4:18">
+    <row r="158" spans="1:16">
       <c r="I158" s="9"/>
-    </row>
-    <row r="159" spans="4:18">
+      <c r="P158" s="15"/>
+    </row>
+    <row r="159" spans="1:16">
       <c r="I159" s="9"/>
-    </row>
-    <row r="160" spans="4:18">
+      <c r="P159" s="15"/>
+    </row>
+    <row r="160" spans="1:16">
+      <c r="D160" s="9"/>
       <c r="I160" s="9"/>
     </row>
-    <row r="161" spans="1:30">
+    <row r="161" spans="4:18">
+      <c r="D161" s="9"/>
       <c r="I161" s="9"/>
     </row>
-    <row r="162" spans="1:30">
+    <row r="162" spans="4:18">
+      <c r="D162" s="9"/>
       <c r="I162" s="9"/>
     </row>
-    <row r="163" spans="1:30">
+    <row r="163" spans="4:18">
+      <c r="D163" s="9"/>
       <c r="I163" s="9"/>
     </row>
-    <row r="164" spans="1:30">
+    <row r="164" spans="4:18">
+      <c r="D164" s="9"/>
       <c r="I164" s="9"/>
     </row>
-    <row r="165" spans="1:30">
+    <row r="165" spans="4:18">
+      <c r="D165" s="9"/>
       <c r="I165" s="9"/>
-      <c r="P165" s="19"/>
-    </row>
-    <row r="166" spans="1:30">
+      <c r="R165" s="17"/>
+    </row>
+    <row r="166" spans="4:18">
       <c r="D166" s="9"/>
       <c r="I166" s="9"/>
     </row>
-    <row r="167" spans="1:30" s="16" customFormat="1">
-      <c r="A167"/>
-      <c r="B167"/>
-      <c r="C167"/>
-      <c r="D167"/>
-      <c r="E167"/>
-      <c r="F167"/>
-      <c r="G167"/>
-      <c r="H167"/>
-      <c r="I167"/>
-      <c r="J167"/>
-      <c r="K167"/>
-      <c r="L167"/>
-      <c r="M167"/>
-      <c r="N167"/>
-      <c r="O167"/>
-      <c r="P167"/>
-      <c r="Q167" s="1"/>
-      <c r="R167"/>
-      <c r="S167"/>
-      <c r="T167"/>
-      <c r="U167"/>
-      <c r="V167"/>
-      <c r="W167"/>
-      <c r="X167"/>
-      <c r="Y167"/>
-      <c r="Z167"/>
-      <c r="AA167"/>
-      <c r="AB167"/>
-      <c r="AC167"/>
-      <c r="AD167"/>
-    </row>
-    <row r="169" spans="1:30">
+    <row r="167" spans="4:18">
+      <c r="D167" s="9"/>
+      <c r="I167" s="9"/>
+      <c r="P167" s="18"/>
+    </row>
+    <row r="168" spans="4:18">
+      <c r="I168" s="9"/>
+    </row>
+    <row r="169" spans="4:18">
       <c r="I169" s="9"/>
-      <c r="P169" s="18"/>
-    </row>
-    <row r="170" spans="1:30">
-      <c r="D170" s="9"/>
-    </row>
-    <row r="173" spans="1:30">
-      <c r="D173" s="9"/>
+    </row>
+    <row r="170" spans="4:18">
+      <c r="I170" s="9"/>
+    </row>
+    <row r="171" spans="4:18">
+      <c r="I171" s="9"/>
+    </row>
+    <row r="172" spans="4:18">
+      <c r="I172" s="9"/>
+    </row>
+    <row r="173" spans="4:18">
       <c r="I173" s="9"/>
     </row>
-    <row r="174" spans="1:30">
+    <row r="174" spans="4:18">
       <c r="I174" s="9"/>
     </row>
-    <row r="175" spans="1:30">
-      <c r="D175" s="9"/>
+    <row r="175" spans="4:18">
+      <c r="I175" s="9"/>
+    </row>
+    <row r="176" spans="4:18">
+      <c r="I176" s="9"/>
+    </row>
+    <row r="177" spans="1:30">
+      <c r="I177" s="9"/>
+    </row>
+    <row r="178" spans="1:30">
+      <c r="I178" s="9"/>
+      <c r="P178" s="19"/>
+    </row>
+    <row r="179" spans="1:30">
+      <c r="D179" s="9"/>
+      <c r="I179" s="9"/>
+    </row>
+    <row r="180" spans="1:30" s="16" customFormat="1">
+      <c r="A180"/>
+      <c r="B180"/>
+      <c r="C180"/>
+      <c r="D180"/>
+      <c r="E180"/>
+      <c r="F180"/>
+      <c r="G180"/>
+      <c r="H180"/>
+      <c r="I180"/>
+      <c r="J180"/>
+      <c r="K180"/>
+      <c r="L180"/>
+      <c r="M180"/>
+      <c r="N180"/>
+      <c r="O180"/>
+      <c r="P180"/>
+      <c r="Q180" s="1"/>
+      <c r="R180"/>
+      <c r="S180"/>
+      <c r="T180"/>
+      <c r="U180"/>
+      <c r="V180"/>
+      <c r="W180"/>
+      <c r="X180"/>
+      <c r="Y180"/>
+      <c r="Z180"/>
+      <c r="AA180"/>
+      <c r="AB180"/>
+      <c r="AC180"/>
+      <c r="AD180"/>
+    </row>
+    <row r="182" spans="1:30">
+      <c r="I182" s="9"/>
+      <c r="P182" s="18"/>
+    </row>
+    <row r="183" spans="1:30">
+      <c r="D183" s="9"/>
+    </row>
+    <row r="186" spans="1:30">
+      <c r="D186" s="9"/>
+      <c r="I186" s="9"/>
+    </row>
+    <row r="187" spans="1:30">
+      <c r="I187" s="9"/>
+    </row>
+    <row r="188" spans="1:30">
+      <c r="D188" s="9"/>
     </row>
   </sheetData>
   <sortState ref="A3:AD178">
@@ -6154,16 +6362,16 @@
     <mergeCell ref="M1:O1"/>
   </mergeCells>
   <dataValidations count="10">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B116 B139:B301">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B116 B152:B314">
       <formula1>$AB$1:$AE$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C116 C139:C301">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C116 C152:C314">
       <formula1>$AB$2:$AE$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C11 C13:C22 C24:C27 C30:C37 C40:C55 C57:C86 C88 C91:C115 C117:C138">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C11 C13:C22 C24:C27 C30:C37 C40:C55 C57:C86 C88 C91:C115 C117:C151">
       <formula1>$AC$1:$AC$9</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B11 B13:B22 B24:B27 B30:B37 B40:B55 B57:B86 B88 B91:B115 B117:B138">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B11 B13:B22 B24:B27 B30:B37 B40:B55 B57:B86 B88 B91:B115 B117:B151">
       <formula1>$AB$1:$AB$9</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23 B29">

</xml_diff>

<commit_message>
Removing unneeded reference files
</commit_message>
<xml_diff>
--- a/assay_data/KlebSeq_assays.xlsx
+++ b/assay_data/KlebSeq_assays.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="36560" windowHeight="23020" tabRatio="500"/>
+    <workbookView xWindow="9180" yWindow="10360" windowWidth="31860" windowHeight="19140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Assays" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="475">
   <si>
     <t>Assay Name</t>
   </si>
@@ -408,30 +408,18 @@
     <t>qnrB</t>
   </si>
   <si>
-    <t>references/qnrB-C1_reference.fasta</t>
-  </si>
-  <si>
     <t>qnrB-C2_UT1</t>
   </si>
   <si>
-    <t>references/qnrB-C2_reference.fasta</t>
-  </si>
-  <si>
     <t>qnrB-C3_UT2</t>
   </si>
   <si>
-    <t>references/qnrB-C3_reference.fasta</t>
-  </si>
-  <si>
     <t>CTX-M-G1_64_UT1</t>
   </si>
   <si>
     <t>blaCTX-M</t>
   </si>
   <si>
-    <t>references/CTX-M-G1_64_reference.fasta</t>
-  </si>
-  <si>
     <t>ESBL present- resistant to extended-spectrum cephalosporins (e.g., cefotaxime amd ceftazidime) ansd monobactams (e.g., aztreonam)</t>
   </si>
   <si>
@@ -444,18 +432,12 @@
     <t>CTX-M-G2_74-75_UT1</t>
   </si>
   <si>
-    <t>references/CTX-M-G2_74-75_reference.fasta</t>
-  </si>
-  <si>
     <t>CTX-M-G2_74-75_UT2</t>
   </si>
   <si>
     <t>CTX-M-G8_G25_UT1</t>
   </si>
   <si>
-    <t>references/CTX-M-G8_25_reference.fasta</t>
-  </si>
-  <si>
     <t>CTX-M-G8_G25_UT2</t>
   </si>
   <si>
@@ -498,21 +480,12 @@
     <t>dfrA14-30_UT2</t>
   </si>
   <si>
-    <t>references/dfrA14-30_reference.fasta</t>
-  </si>
-  <si>
     <t>dfrA6-31_UT1</t>
   </si>
   <si>
-    <t>references/dfrA6-31_reference.fasta</t>
-  </si>
-  <si>
     <t>dfrA26-13_UT1</t>
   </si>
   <si>
-    <t>references/dfrA26-13_reference.fasta</t>
-  </si>
-  <si>
     <t>dfrA8_UT1</t>
   </si>
   <si>
@@ -609,21 +582,12 @@
     <t>dfrB</t>
   </si>
   <si>
-    <t>references/dfrB1-8_reference.fasta</t>
-  </si>
-  <si>
     <t>dfrB2-7_UT1</t>
   </si>
   <si>
-    <t>references/dfrB2-7_reference.fasta</t>
-  </si>
-  <si>
     <t>dfrB3_1_UT1</t>
   </si>
   <si>
-    <t>AC-----CCGACAACTTGACCCTGCCAAGCGGCGCCAGATTTCTTG-------CGCACGCGATCTCCC-----AGGCCAAAC-GTGGCGTGCGATGGGAGCGCAAACTGGC-CAGCAACTAGAGT-ACTGACTCCATTGTTGTGTT------GGT</t>
-  </si>
-  <si>
     <t>dfrB4_UT1</t>
   </si>
   <si>
@@ -834,18 +798,12 @@
     <t>acetyltransferase</t>
   </si>
   <si>
-    <t>references/aac6-Ib_reference.fasta</t>
-  </si>
-  <si>
     <t>Tobramycin and amikacin resistance OR fluoroquinolone resistance</t>
   </si>
   <si>
     <t>aac3-II_UT</t>
   </si>
   <si>
-    <t>references/aac3-II_reference.fasta</t>
-  </si>
-  <si>
     <t>Gentamicin and tobramycin resistance</t>
   </si>
   <si>
@@ -867,18 +825,12 @@
     <t>adenylyltransferase</t>
   </si>
   <si>
-    <t>references/aadB_reference.fasta</t>
-  </si>
-  <si>
     <t>Gentamicin, tobramycin, and kanamycin resistance</t>
   </si>
   <si>
     <t>aadA_UT</t>
   </si>
   <si>
-    <t>references/aadA_reference.fasta</t>
-  </si>
-  <si>
     <t>Streptomycin and spectinomycin resistance</t>
   </si>
   <si>
@@ -888,9 +840,6 @@
     <t>aminoglycoside response regulator</t>
   </si>
   <si>
-    <t>CCACGGCGCTTTAAGTCCTCCAACGAATCCAACATTCCCCTTATTAATTCAACAGGATGCCCCTCCCAGTCTTCAACAACGCCMACAATTCTCAAGGGTTCGCAGGTTCTATAGGACTGTGTTGGATTACCGGGAAATCTTTTGTTCGTAAGATTCGGATCGTCTTCGAACGGTCCTGTTGGCTCAACTATGTATATGTAGCCGCGACCCTCGAGGCCAGACAGTGACATAGCAAGTTCAGCTCC</t>
-  </si>
-  <si>
     <t>Aminoglycoside resistance</t>
   </si>
   <si>
@@ -906,9 +855,6 @@
     <t>cat gene</t>
   </si>
   <si>
-    <t>references/catA_reference.fasta</t>
-  </si>
-  <si>
     <t>Chloramphenicol resistance</t>
   </si>
   <si>
@@ -918,18 +864,12 @@
     <t>cml genes</t>
   </si>
   <si>
-    <t>references/cmlA-B_reference.fasta</t>
-  </si>
-  <si>
     <t>floR_UT</t>
   </si>
   <si>
     <t>floR</t>
   </si>
   <si>
-    <t>references/floR_reference.fasta</t>
-  </si>
-  <si>
     <t>mphA_UT</t>
   </si>
   <si>
@@ -948,9 +888,6 @@
     <t>strA gene</t>
   </si>
   <si>
-    <t>references/strA_reference.fasta</t>
-  </si>
-  <si>
     <t>Streptomycin resistance</t>
   </si>
   <si>
@@ -960,9 +897,6 @@
     <t>strB gene</t>
   </si>
   <si>
-    <t>references/strB_reference.fasta</t>
-  </si>
-  <si>
     <t>mcr-1_UT</t>
   </si>
   <si>
@@ -981,9 +915,6 @@
     <t>tetA</t>
   </si>
   <si>
-    <t>references/tetA_reference.fasta</t>
-  </si>
-  <si>
     <t>Tetracycline resistance</t>
   </si>
   <si>
@@ -993,27 +924,18 @@
     <t>tetB</t>
   </si>
   <si>
-    <t>references/tetB_reference.fasta</t>
-  </si>
-  <si>
     <t>tetG_UT</t>
   </si>
   <si>
     <t>tetG</t>
   </si>
   <si>
-    <t>references/tetG_reference.fasta</t>
-  </si>
-  <si>
     <t>tetD_UT</t>
   </si>
   <si>
     <t>tetD</t>
   </si>
   <si>
-    <t>references/tetD_reference.fasta</t>
-  </si>
-  <si>
     <t>ST395_UT</t>
   </si>
   <si>
@@ -1281,9 +1203,6 @@
     <t>Klebsiella pneumoniae CG14 present</t>
   </si>
   <si>
-    <t>CG101_UT?</t>
-  </si>
-  <si>
     <t>inST14_UT</t>
   </si>
   <si>
@@ -1443,19 +1362,10 @@
     <t>Kquasi_UT</t>
   </si>
   <si>
-    <t>GCCATGATGCAGCCTTTGCCGGCCATCGACAGCATCTCrGCGTCGTTCATACCGTCGCCGAAGGCGATGCAATCGGCAAGAGTGTAACCGAGCATTTTCGCCACCGCCTCCAGCGCATGCCCCTTCGATACCCCACCCGCCATGACTTCCAGGCAGGTTAAGGTGGAGAAGCTGACGTTCACGCGAT</t>
-  </si>
-  <si>
-    <t>Klebsiella quasipnuemoniae present</t>
-  </si>
-  <si>
     <t>blaVIM_UT</t>
   </si>
   <si>
     <t>blaVIM</t>
-  </si>
-  <si>
-    <t>GGCGGCGTTGATGTCCTTCGGGCGGCTGGGGTGGCAACGTACGCATCACCGTCGACACGCCGGCTAGCCGAGGTAGAGGGGAACGAGATTCCCACGCACTCTCTAGAAGGACTCTCATCGAGCGGGGACGCAGTGCGCTTCGGTCCAGTAGAACTCTTCTATCCTGGTGCTGCGCATTCGACCGACAACTTAGTTGTGTACGTCCCGTCTGCGAGTGTGCTCTATGGTGGTTGTGCG</t>
   </si>
   <si>
     <r>
@@ -1484,9 +1394,6 @@
     <t>blaGES</t>
   </si>
   <si>
-    <t>GGTGCAGCTTAGCGACAATGGGGCTACTAACCTCTTACTGAGAGAAATTGGCGGACCTGCTGCAATGACGCAGTATTTTCGTAAAATTGGCGACTCTGTGAGTCGGCTAGACCGGAAAGAGCCGGAGATGGGCGACAACACACCTGGCGACCTCAGAGATACAACTACGCCTATTGCTATGGCACGTACTGTGGCTAAAGTCCTCTATGGCGGCGCACTGACGTCCACTTCGACCCACACCATTGAGAGGTGGCTGATCGGAAACCAAACGGGAG</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -1503,9 +1410,6 @@
   </si>
   <si>
     <t>blaOXA-48 group</t>
-  </si>
-  <si>
-    <t>references/blaOXA-48_reference.fasta</t>
   </si>
   <si>
     <r>
@@ -1534,10 +1438,154 @@
     <t>fosA</t>
   </si>
   <si>
-    <t>references/fosA_reference.fasta</t>
-  </si>
-  <si>
     <t>Fosfomycin resistance</t>
+  </si>
+  <si>
+    <t>CTTCAGCTATCGCCTGGAGTGCTATACCCCGGCGCCGAAGCGGCAGTATGGCTACTTCGTACTGCCCCTGCTGCACCAGGGGAAACTGGTTGGGCGGATGGACAGTAAAATGCATCGCAAAAGCCAGGAGCTGGAGATCTTCTCCCTGTGGCTGGAGGATGAGGTGAAGATCACCCGTGGCCTTGAGCAGGGGCTGCGCCGGGCGATCAACGACTTCGCGCGCTGGCAATCGGCGGACCGGATCCTGTGTCGACGCCTGCCGGAAGGGCTGTTTGTCGGCCAGGAGC</t>
+  </si>
+  <si>
+    <t>GCCATGATGCAGCCTTTGCCGGCCATCGACAGCATCTCGGCGTCGTTCATGCCGTCGCCGAAAGCGATGCAATCGGCCAGACTGTAACCGAGCATTTTCGCCACCGCCTCCAGCGCATGCCCCTTCGATACCCCACCCGCCATGACCTCCAGGCAGGTTAAGGTGGAGAAGCTGACGTTCACGCGAT</t>
+  </si>
+  <si>
+    <t>GCCATGATGCAGCCTTTGCCGGCCATCGACAGCATCTCAGCGTCGTTCATACCGTCGCCGAAGGCGATGCAATCGGCAAGAGTGTAACCGAGCATTTTCGCCACCGCCTCCAGCGCATGCCCCTTCGATACCCCACCCGCCATGACTTCCAGGCAGGTTAAGGTGGAGAAGCTGACGTTCACGCGAT</t>
+  </si>
+  <si>
+    <t>Klebsiella pneumoniae or quasipneumoniae present</t>
+  </si>
+  <si>
+    <t>Klebsiella quasipneumoniae present</t>
+  </si>
+  <si>
+    <t>Klebsiella pnuemoniae or variicola present</t>
+  </si>
+  <si>
+    <t>references/qnrB-C1_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/qnrB-C2_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/qnrB-C3_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>CCGTCACGCTGTTGTTAGGAAGTGTGCCGCTGTATGCGCAAACGGCGGACGTACAGCAAAAACTTGCCGAATTAGAGCGGCAGTCGGGAGGCAGACTGGGTGTGGCATTGATTAACACAGCAGATAATTCGCAAATACTTTATCGTGCTGATGAGCG</t>
+  </si>
+  <si>
+    <t>references/CTX-M-G2_UT1amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/CTX-M-G2_UT2amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/CTX-M-G8_G25_UT1amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/CTX-M-G8_G25_UT2amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/dfrA14-30_UT2_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/dfrA6-31_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/dfrA26-13_UT1_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/dfrB1-8_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/dfrB2-7_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/dfrB3_1_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/aac6-Ibamplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/aac3-IIamplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/aadB_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/aadA_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/catA_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/cmlA-B_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/floR_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/strA_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/strB_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/tetA_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/tetB_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/tetG_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/tetD_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/blaOXA-48amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/fosA_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/blaVIM_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>references/blaGES_amplicons_derep.fasta</t>
+  </si>
+  <si>
+    <t>CG43_UT</t>
+  </si>
+  <si>
+    <t>KP1_1248</t>
+  </si>
+  <si>
+    <t>GGrCCCAGCTATGTGCTTGGCGATCTGGCCACCCATCCGCTGTTTGTCGCCGAGACCATGGCGCCGCAGCTCAATATCAAACGGCTGATGTGCTCCCGTCAGAGCTTTGTTCCCTCCCGCGCGCCGCTGGAAGATAACGCCTTTGTCCTGATGGAATATGACAACGGCGCGGTTGGCTCGATGTGGACCAGCGCGGTCAACAGCGGCGCCATGCACTCGCAAAAAGTGCGCATCGTCGGCGAAAAAGCAAGCATyGAATGGTGG</t>
+  </si>
+  <si>
+    <t>Klebsiella pneumoniae CG101 present</t>
+  </si>
+  <si>
+    <t>kvari</t>
+  </si>
+  <si>
+    <t>kquasi</t>
+  </si>
+  <si>
+    <t>not_kquasi</t>
+  </si>
+  <si>
+    <t>not_kvari</t>
+  </si>
+  <si>
+    <t>CCACGGCGCTTTAAGTCCTCCAACGAATCCAACATTCCCCTTATTAATTCAACAGGATGCCCCTCCCAGTCTTCAACAACGCCAACAATTCTCAAGGGTTCGCAGGTTCTATAGGACTGTGTTGGATTACCGGGAAATCTTTTGTTCGTAAGATTCGGATCGTCTTCGAACGGTCCTGTTGGCTCAACTATGTATATGTAGCCGCGACCCTCGAGGCCAGACAGTGACATAGCAAGTTCAGCTCC</t>
+  </si>
+  <si>
+    <t>CCACGACGTTTTAAATCTTCTAATGAATCTAACATTCCTCTTATTAATTCAACAGGATGTCCTTCCCAATCTTCAACAACACCAACAATTCTTAAAGGTTCACAAGTTCTATAAGATTGTGTTGGATTACCAGGAAATTTTTTATTTGTAAGATTTGGATCATCTTCAAATGGTCCTGTTGGTTCAACTATATATATATAACCACGACCTTCAAGACCAGATAGTGACATAGCAAGTTCAGCTCC</t>
+  </si>
+  <si>
+    <t>arr</t>
+  </si>
+  <si>
+    <t>JQ638951.1</t>
   </si>
 </sst>
 </file>
@@ -1719,7 +1767,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="331">
+  <cellStyleXfs count="343">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2026,6 +2074,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2109,7 +2169,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="331">
+  <cellStyles count="343">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2408,6 +2468,12 @@
     <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2439,6 +2505,12 @@
     <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="1" builtinId="25" customBuiltin="1"/>
   </cellStyles>
@@ -2769,10 +2841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE188"/>
+  <dimension ref="A1:AE178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="M153" sqref="M153"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2916,12 +2988,8 @@
       <c r="P3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AB3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC3" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="8"/>
       <c r="AD3" s="6"/>
     </row>
     <row r="4" spans="1:31">
@@ -3346,7 +3414,7 @@
         <v>95</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>96</v>
+        <v>432</v>
       </c>
       <c r="P23" t="s">
         <v>84</v>
@@ -3355,7 +3423,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -3367,7 +3435,7 @@
         <v>95</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>98</v>
+        <v>433</v>
       </c>
       <c r="P24" t="s">
         <v>84</v>
@@ -3375,7 +3443,7 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
@@ -3387,7 +3455,7 @@
         <v>95</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>100</v>
+        <v>434</v>
       </c>
       <c r="P25" t="s">
         <v>84</v>
@@ -3395,27 +3463,27 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
         <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>103</v>
+        <v>435</v>
       </c>
       <c r="P26" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B27" t="s">
         <v>20</v>
@@ -3424,18 +3492,18 @@
         <v>26</v>
       </c>
       <c r="D27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I27" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="I27" s="9" t="s">
-        <v>106</v>
-      </c>
       <c r="P27" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B28" t="s">
         <v>25</v>
@@ -3444,19 +3512,19 @@
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>108</v>
+        <v>436</v>
       </c>
       <c r="P28" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="Q28"/>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B29" t="s">
         <v>25</v>
@@ -3465,18 +3533,18 @@
         <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>108</v>
+        <v>437</v>
       </c>
       <c r="P29" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
         <v>25</v>
@@ -3485,18 +3553,18 @@
         <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>111</v>
+        <v>438</v>
       </c>
       <c r="P30" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B31" t="s">
         <v>25</v>
@@ -3505,18 +3573,18 @@
         <v>26</v>
       </c>
       <c r="D31" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>111</v>
+        <v>439</v>
       </c>
       <c r="P31" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B32" t="s">
         <v>20</v>
@@ -3525,18 +3593,18 @@
         <v>26</v>
       </c>
       <c r="D32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="P32" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:17">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B33" t="s">
         <v>20</v>
@@ -3545,18 +3613,18 @@
         <v>26</v>
       </c>
       <c r="D33" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="P33" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:17">
       <c r="A34" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B34" t="s">
         <v>20</v>
@@ -3565,18 +3633,18 @@
         <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="P34" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:17">
       <c r="A35" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B35" t="s">
         <v>20</v>
@@ -3585,18 +3653,18 @@
         <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="P35" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:17">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B36" t="s">
         <v>20</v>
@@ -3605,18 +3673,18 @@
         <v>26</v>
       </c>
       <c r="D36" t="s">
+        <v>112</v>
+      </c>
+      <c r="I36" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="I36" s="9" t="s">
-        <v>124</v>
-      </c>
       <c r="P36" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:17">
       <c r="A37" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B37" t="s">
         <v>25</v>
@@ -3625,18 +3693,18 @@
         <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I37" s="9" t="s">
-        <v>126</v>
+        <v>440</v>
       </c>
       <c r="P37" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:17">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B38" t="s">
         <v>25</v>
@@ -3645,19 +3713,19 @@
         <v>26</v>
       </c>
       <c r="D38" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>128</v>
+        <v>441</v>
       </c>
       <c r="P38" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="Q38"/>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B39" t="s">
         <v>25</v>
@@ -3666,19 +3734,19 @@
         <v>26</v>
       </c>
       <c r="D39" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>130</v>
+        <v>442</v>
       </c>
       <c r="P39" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="Q39"/>
     </row>
     <row r="40" spans="1:17">
       <c r="A40" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B40" t="s">
         <v>20</v>
@@ -3687,18 +3755,18 @@
         <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="P40" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:17">
       <c r="A41" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B41" t="s">
         <v>20</v>
@@ -3707,18 +3775,18 @@
         <v>26</v>
       </c>
       <c r="D41" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="P41" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:17">
       <c r="A42" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B42" t="s">
         <v>20</v>
@@ -3727,18 +3795,18 @@
         <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="P42" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:17">
       <c r="A43" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B43" t="s">
         <v>20</v>
@@ -3747,18 +3815,18 @@
         <v>26</v>
       </c>
       <c r="D43" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I43" s="9" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="P43" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:17">
       <c r="A44" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B44" t="s">
         <v>20</v>
@@ -3767,18 +3835,18 @@
         <v>26</v>
       </c>
       <c r="D44" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="P44" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:17">
       <c r="A45" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B45" t="s">
         <v>20</v>
@@ -3787,18 +3855,18 @@
         <v>26</v>
       </c>
       <c r="D45" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I45" s="9" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="P45" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:17">
       <c r="A46" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B46" t="s">
         <v>20</v>
@@ -3807,18 +3875,18 @@
         <v>26</v>
       </c>
       <c r="D46" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I46" s="9" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="P46" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:17">
       <c r="A47" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B47" t="s">
         <v>20</v>
@@ -3827,18 +3895,18 @@
         <v>26</v>
       </c>
       <c r="D47" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I47" s="9" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="P47" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:17">
       <c r="A48" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B48" t="s">
         <v>20</v>
@@ -3847,18 +3915,18 @@
         <v>26</v>
       </c>
       <c r="D48" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I48" s="9" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="P48" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:17">
       <c r="A49" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B49" t="s">
         <v>20</v>
@@ -3867,18 +3935,18 @@
         <v>26</v>
       </c>
       <c r="D49" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="P49" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:17">
       <c r="A50" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B50" t="s">
         <v>20</v>
@@ -3887,18 +3955,18 @@
         <v>26</v>
       </c>
       <c r="D50" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I50" s="9" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="P50" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:17">
       <c r="A51" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B51" t="s">
         <v>20</v>
@@ -3907,18 +3975,18 @@
         <v>26</v>
       </c>
       <c r="D51" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I51" s="9" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="P51" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:17">
       <c r="A52" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B52" t="s">
         <v>20</v>
@@ -3927,18 +3995,18 @@
         <v>26</v>
       </c>
       <c r="D52" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I52" s="9" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="P52" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:17">
       <c r="A53" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B53" t="s">
         <v>20</v>
@@ -3947,18 +4015,18 @@
         <v>26</v>
       </c>
       <c r="D53" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I53" s="9" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="P53" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:17">
       <c r="A54" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B54" t="s">
         <v>20</v>
@@ -3967,18 +4035,18 @@
         <v>26</v>
       </c>
       <c r="D54" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I54" s="9" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="P54" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:17">
       <c r="A55" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B55" t="s">
         <v>25</v>
@@ -3987,18 +4055,18 @@
         <v>26</v>
       </c>
       <c r="D55" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="I55" s="9" t="s">
-        <v>163</v>
+        <v>443</v>
       </c>
       <c r="P55" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:17">
       <c r="A56" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B56" t="s">
         <v>25</v>
@@ -4007,39 +4075,39 @@
         <v>26</v>
       </c>
       <c r="D56" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="I56" s="9" t="s">
-        <v>165</v>
+        <v>444</v>
       </c>
       <c r="P56" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="Q56"/>
     </row>
     <row r="57" spans="1:17">
       <c r="A57" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B57" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C57" t="s">
         <v>26</v>
       </c>
       <c r="D57" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="I57" s="9" t="s">
-        <v>167</v>
+        <v>445</v>
       </c>
       <c r="P57" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:17">
       <c r="A58" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B58" t="s">
         <v>20</v>
@@ -4048,18 +4116,18 @@
         <v>26</v>
       </c>
       <c r="D58" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="I58" s="9" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="P58" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:17">
       <c r="A59" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="B59" t="s">
         <v>20</v>
@@ -4068,18 +4136,18 @@
         <v>26</v>
       </c>
       <c r="D59" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="I59" s="9" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="P59" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:17">
       <c r="A60" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="B60" t="s">
         <v>20</v>
@@ -4088,18 +4156,18 @@
         <v>26</v>
       </c>
       <c r="D60" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="I60" s="9" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="P60" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:17">
       <c r="A61" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="B61" t="s">
         <v>20</v>
@@ -4108,18 +4176,18 @@
         <v>26</v>
       </c>
       <c r="D61" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="P61" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:17">
       <c r="A62" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="B62" t="s">
         <v>21</v>
@@ -4128,27 +4196,27 @@
         <v>23</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="I62" s="9" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="J62">
         <v>35</v>
       </c>
       <c r="K62" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="L62" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="P62" s="18" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:17">
       <c r="A63" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="B63" t="s">
         <v>25</v>
@@ -4157,18 +4225,18 @@
         <v>23</v>
       </c>
       <c r="D63" s="21" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="I63" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="P63" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="1:17">
       <c r="A64" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B64" t="s">
         <v>20</v>
@@ -4177,18 +4245,18 @@
         <v>28</v>
       </c>
       <c r="D64" s="21" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="I64" s="9" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="P64" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
     </row>
     <row r="65" spans="1:29">
       <c r="A65" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="B65" t="s">
         <v>20</v>
@@ -4197,18 +4265,18 @@
         <v>28</v>
       </c>
       <c r="D65" s="21" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="I65" s="9" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="P65" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
     </row>
     <row r="66" spans="1:29">
       <c r="A66" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="B66" t="s">
         <v>20</v>
@@ -4217,18 +4285,18 @@
         <v>28</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="I66" s="9" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="P66" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
     </row>
     <row r="67" spans="1:29">
       <c r="A67" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="B67" t="s">
         <v>20</v>
@@ -4237,18 +4305,18 @@
         <v>28</v>
       </c>
       <c r="D67" s="21" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="I67" s="9" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="P67" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
     </row>
     <row r="68" spans="1:29">
       <c r="A68" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="B68" t="s">
         <v>20</v>
@@ -4257,18 +4325,18 @@
         <v>28</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="I68" s="9" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="P68" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
     <row r="69" spans="1:29">
       <c r="A69" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="B69" t="s">
         <v>20</v>
@@ -4277,18 +4345,18 @@
         <v>28</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="I69" s="9" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="P69" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="70" spans="1:29">
       <c r="A70" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="B70" t="s">
         <v>20</v>
@@ -4297,18 +4365,18 @@
         <v>28</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="I70" s="9" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="P70" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="71" spans="1:29">
       <c r="A71" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="B71" t="s">
         <v>20</v>
@@ -4317,18 +4385,18 @@
         <v>28</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="I71" s="9" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="P71" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="72" spans="1:29">
       <c r="A72" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="B72" t="s">
         <v>20</v>
@@ -4337,18 +4405,18 @@
         <v>28</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="I72" s="9" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P72" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="1:29">
       <c r="A73" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B73" t="s">
         <v>20</v>
@@ -4357,18 +4425,18 @@
         <v>28</v>
       </c>
       <c r="D73" s="21" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="I73" s="9" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="P73" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
     </row>
     <row r="74" spans="1:29">
       <c r="A74" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B74" t="s">
         <v>20</v>
@@ -4377,18 +4445,18 @@
         <v>28</v>
       </c>
       <c r="D74" s="21" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="I74" s="9" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="P74" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
     </row>
     <row r="75" spans="1:29">
       <c r="A75" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="B75" t="s">
         <v>20</v>
@@ -4397,18 +4465,18 @@
         <v>28</v>
       </c>
       <c r="D75" s="21" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="I75" s="9" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="P75" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="76" spans="1:29">
       <c r="A76" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="B76" t="s">
         <v>20</v>
@@ -4417,18 +4485,18 @@
         <v>28</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="I76" s="9" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="P76" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
     </row>
     <row r="77" spans="1:29">
       <c r="A77" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="B77" t="s">
         <v>20</v>
@@ -4437,18 +4505,18 @@
         <v>28</v>
       </c>
       <c r="D77" s="21" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="I77" s="9" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="P77" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
     </row>
     <row r="78" spans="1:29">
       <c r="A78" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="B78" t="s">
         <v>25</v>
@@ -4457,18 +4525,18 @@
         <v>26</v>
       </c>
       <c r="D78" s="21" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="I78" s="9" t="s">
-        <v>238</v>
+        <v>446</v>
       </c>
       <c r="P78" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:29">
       <c r="A79" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="B79" t="s">
         <v>25</v>
@@ -4477,13 +4545,13 @@
         <v>26</v>
       </c>
       <c r="D79" s="21" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="I79" s="9" t="s">
-        <v>241</v>
+        <v>447</v>
       </c>
       <c r="P79" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="AB79" s="20" t="s">
         <v>27</v>
@@ -4494,7 +4562,7 @@
     </row>
     <row r="80" spans="1:29">
       <c r="A80" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="B80" t="s">
         <v>20</v>
@@ -4503,18 +4571,18 @@
         <v>26</v>
       </c>
       <c r="D80" s="21" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="I80" s="9" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="P80" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
     </row>
     <row r="81" spans="1:16">
       <c r="A81" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="B81" t="s">
         <v>25</v>
@@ -4523,18 +4591,18 @@
         <v>26</v>
       </c>
       <c r="D81" s="21" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="I81" s="9" t="s">
-        <v>249</v>
+        <v>448</v>
       </c>
       <c r="P81" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
     </row>
     <row r="82" spans="1:16">
       <c r="A82" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B82" t="s">
         <v>25</v>
@@ -4543,78 +4611,73 @@
         <v>26</v>
       </c>
       <c r="D82" s="21" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="I82" s="9" t="s">
-        <v>252</v>
+        <v>449</v>
       </c>
       <c r="P82" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
     </row>
     <row r="83" spans="1:16">
       <c r="A83" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="B83" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C83" t="s">
         <v>26</v>
       </c>
       <c r="D83" s="21" t="s">
-        <v>255</v>
+        <v>239</v>
+      </c>
+      <c r="H83" t="s">
+        <v>473</v>
       </c>
       <c r="I83" s="9" t="s">
-        <v>256</v>
+        <v>471</v>
       </c>
       <c r="P83" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
     </row>
     <row r="84" spans="1:16">
-      <c r="A84" t="s">
-        <v>258</v>
-      </c>
-      <c r="B84" t="s">
-        <v>20</v>
-      </c>
-      <c r="C84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D84" s="21" t="s">
-        <v>248</v>
+      <c r="D84" s="21"/>
+      <c r="H84" t="s">
+        <v>474</v>
       </c>
       <c r="I84" s="9" t="s">
-        <v>259</v>
+        <v>472</v>
       </c>
       <c r="P84" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
     </row>
     <row r="85" spans="1:16">
       <c r="A85" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="B85" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C85" t="s">
         <v>26</v>
       </c>
       <c r="D85" s="21" t="s">
-        <v>261</v>
+        <v>234</v>
       </c>
       <c r="I85" s="9" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="P85" t="s">
-        <v>263</v>
+        <v>237</v>
       </c>
     </row>
     <row r="86" spans="1:16">
       <c r="A86" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="B86" t="s">
         <v>25</v>
@@ -4623,18 +4686,18 @@
         <v>26</v>
       </c>
       <c r="D86" s="21" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="I86" s="9" t="s">
-        <v>266</v>
+        <v>450</v>
       </c>
       <c r="P86" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
     </row>
     <row r="87" spans="1:16">
       <c r="A87" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="B87" t="s">
         <v>25</v>
@@ -4643,58 +4706,58 @@
         <v>26</v>
       </c>
       <c r="D87" s="21" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="I87" s="9" t="s">
-        <v>269</v>
+        <v>451</v>
       </c>
       <c r="P87" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
     </row>
     <row r="88" spans="1:16">
       <c r="A88" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="B88" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C88" t="s">
         <v>26</v>
       </c>
       <c r="D88" s="21" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
       <c r="I88" s="9" t="s">
-        <v>272</v>
+        <v>452</v>
       </c>
       <c r="P88" t="s">
-        <v>273</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89" spans="1:16">
       <c r="A89" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="B89" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C89" t="s">
         <v>26</v>
       </c>
       <c r="D89" s="21" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="I89" s="9" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="P89" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
     </row>
     <row r="90" spans="1:16">
       <c r="A90" t="s">
-        <v>278</v>
+        <v>254</v>
       </c>
       <c r="B90" t="s">
         <v>25</v>
@@ -4703,58 +4766,58 @@
         <v>26</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="I90" s="9" t="s">
-        <v>280</v>
+        <v>453</v>
       </c>
       <c r="P90" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
     </row>
     <row r="91" spans="1:16">
       <c r="A91" t="s">
-        <v>281</v>
+        <v>257</v>
       </c>
       <c r="B91" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C91" t="s">
         <v>26</v>
       </c>
       <c r="D91" s="21" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="I91" s="9" t="s">
-        <v>283</v>
+        <v>454</v>
       </c>
       <c r="P91" t="s">
-        <v>284</v>
+        <v>256</v>
       </c>
     </row>
     <row r="92" spans="1:16">
       <c r="A92" t="s">
-        <v>285</v>
+        <v>259</v>
       </c>
       <c r="B92" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C92" t="s">
         <v>26</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>286</v>
+        <v>260</v>
       </c>
       <c r="I92" s="9" t="s">
-        <v>287</v>
+        <v>261</v>
       </c>
       <c r="P92" t="s">
-        <v>288</v>
+        <v>262</v>
       </c>
     </row>
     <row r="93" spans="1:16">
       <c r="A93" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
       <c r="B93" t="s">
         <v>25</v>
@@ -4763,18 +4826,18 @@
         <v>26</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>290</v>
+        <v>264</v>
       </c>
       <c r="I93" s="9" t="s">
-        <v>291</v>
+        <v>455</v>
       </c>
       <c r="P93" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
     </row>
     <row r="94" spans="1:16">
       <c r="A94" t="s">
-        <v>292</v>
+        <v>266</v>
       </c>
       <c r="B94" t="s">
         <v>25</v>
@@ -4783,18 +4846,18 @@
         <v>26</v>
       </c>
       <c r="D94" s="21" t="s">
-        <v>293</v>
+        <v>267</v>
       </c>
       <c r="I94" s="9" t="s">
-        <v>294</v>
+        <v>456</v>
       </c>
       <c r="P94" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
     </row>
     <row r="95" spans="1:16">
       <c r="A95" t="s">
-        <v>295</v>
+        <v>268</v>
       </c>
       <c r="B95" t="s">
         <v>25</v>
@@ -4803,47 +4866,38 @@
         <v>26</v>
       </c>
       <c r="D95" s="21" t="s">
-        <v>296</v>
+        <v>269</v>
       </c>
       <c r="I95" s="9" t="s">
-        <v>297</v>
+        <v>457</v>
       </c>
       <c r="P95" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
     </row>
     <row r="96" spans="1:16">
       <c r="A96" t="s">
-        <v>298</v>
+        <v>270</v>
       </c>
       <c r="B96" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C96" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D96" s="21" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="I96" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="J96">
-        <v>34</v>
-      </c>
-      <c r="K96" t="s">
-        <v>180</v>
-      </c>
-      <c r="L96" t="s">
-        <v>181</v>
+        <v>458</v>
       </c>
       <c r="P96" t="s">
-        <v>301</v>
+        <v>265</v>
       </c>
     </row>
     <row r="97" spans="1:16">
       <c r="A97" t="s">
-        <v>302</v>
+        <v>272</v>
       </c>
       <c r="B97" t="s">
         <v>21</v>
@@ -4852,27 +4906,27 @@
         <v>23</v>
       </c>
       <c r="D97" s="21" t="s">
-        <v>303</v>
+        <v>273</v>
       </c>
       <c r="I97" s="9" t="s">
-        <v>304</v>
+        <v>274</v>
       </c>
       <c r="J97">
         <v>34</v>
       </c>
       <c r="K97" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="L97" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="P97" t="s">
-        <v>305</v>
+        <v>275</v>
       </c>
     </row>
     <row r="98" spans="1:16">
       <c r="A98" t="s">
-        <v>306</v>
+        <v>276</v>
       </c>
       <c r="B98" t="s">
         <v>21</v>
@@ -4881,27 +4935,27 @@
         <v>23</v>
       </c>
       <c r="D98" s="21" t="s">
-        <v>307</v>
+        <v>277</v>
       </c>
       <c r="I98" s="9" t="s">
-        <v>308</v>
+        <v>278</v>
       </c>
       <c r="J98">
         <v>34</v>
       </c>
       <c r="K98" t="s">
-        <v>309</v>
+        <v>168</v>
       </c>
       <c r="L98" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="P98" t="s">
-        <v>310</v>
+        <v>279</v>
       </c>
     </row>
     <row r="99" spans="1:16">
       <c r="A99" t="s">
-        <v>311</v>
+        <v>280</v>
       </c>
       <c r="B99" t="s">
         <v>21</v>
@@ -4910,27 +4964,27 @@
         <v>23</v>
       </c>
       <c r="D99" s="21" t="s">
-        <v>312</v>
+        <v>281</v>
       </c>
       <c r="I99" s="9" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
       <c r="J99">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="K99" t="s">
-        <v>180</v>
+        <v>283</v>
       </c>
       <c r="L99" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="P99" t="s">
-        <v>314</v>
+        <v>284</v>
       </c>
     </row>
     <row r="100" spans="1:16">
       <c r="A100" t="s">
-        <v>315</v>
+        <v>285</v>
       </c>
       <c r="B100" t="s">
         <v>21</v>
@@ -4939,27 +4993,27 @@
         <v>23</v>
       </c>
       <c r="D100" s="21" t="s">
-        <v>316</v>
+        <v>286</v>
       </c>
       <c r="I100" s="9" t="s">
-        <v>317</v>
+        <v>287</v>
       </c>
       <c r="J100">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="K100" t="s">
-        <v>309</v>
+        <v>168</v>
       </c>
       <c r="L100" t="s">
-        <v>318</v>
+        <v>169</v>
       </c>
       <c r="P100" t="s">
-        <v>319</v>
+        <v>288</v>
       </c>
     </row>
     <row r="101" spans="1:16">
       <c r="A101" t="s">
-        <v>320</v>
+        <v>289</v>
       </c>
       <c r="B101" t="s">
         <v>21</v>
@@ -4968,27 +5022,27 @@
         <v>23</v>
       </c>
       <c r="D101" s="21" t="s">
-        <v>321</v>
+        <v>290</v>
       </c>
       <c r="I101" s="9" t="s">
-        <v>322</v>
+        <v>291</v>
       </c>
       <c r="J101">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="K101" t="s">
-        <v>180</v>
+        <v>283</v>
       </c>
       <c r="L101" t="s">
-        <v>181</v>
+        <v>292</v>
       </c>
       <c r="P101" t="s">
-        <v>323</v>
+        <v>293</v>
       </c>
     </row>
     <row r="102" spans="1:16">
       <c r="A102" t="s">
-        <v>324</v>
+        <v>294</v>
       </c>
       <c r="B102" t="s">
         <v>21</v>
@@ -4997,27 +5051,27 @@
         <v>23</v>
       </c>
       <c r="D102" s="21" t="s">
-        <v>321</v>
+        <v>295</v>
       </c>
       <c r="I102" s="9" t="s">
-        <v>325</v>
+        <v>296</v>
       </c>
       <c r="J102">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K102" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="L102" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="P102" t="s">
-        <v>326</v>
+        <v>297</v>
       </c>
     </row>
     <row r="103" spans="1:16">
       <c r="A103" t="s">
-        <v>327</v>
+        <v>298</v>
       </c>
       <c r="B103" t="s">
         <v>21</v>
@@ -5026,27 +5080,27 @@
         <v>23</v>
       </c>
       <c r="D103" s="21" t="s">
-        <v>328</v>
+        <v>295</v>
       </c>
       <c r="I103" s="9" t="s">
-        <v>329</v>
+        <v>299</v>
       </c>
       <c r="J103">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="K103" t="s">
-        <v>309</v>
+        <v>168</v>
       </c>
       <c r="L103" t="s">
-        <v>318</v>
+        <v>169</v>
       </c>
       <c r="P103" t="s">
-        <v>330</v>
+        <v>300</v>
       </c>
     </row>
     <row r="104" spans="1:16">
       <c r="A104" t="s">
-        <v>331</v>
+        <v>301</v>
       </c>
       <c r="B104" t="s">
         <v>21</v>
@@ -5055,27 +5109,27 @@
         <v>23</v>
       </c>
       <c r="D104" s="21" t="s">
-        <v>332</v>
+        <v>302</v>
       </c>
       <c r="I104" s="9" t="s">
-        <v>333</v>
+        <v>303</v>
       </c>
       <c r="J104">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="K104" t="s">
-        <v>309</v>
+        <v>283</v>
       </c>
       <c r="L104" t="s">
-        <v>318</v>
+        <v>292</v>
       </c>
       <c r="P104" t="s">
-        <v>334</v>
+        <v>304</v>
       </c>
     </row>
     <row r="105" spans="1:16">
       <c r="A105" t="s">
-        <v>335</v>
+        <v>305</v>
       </c>
       <c r="B105" t="s">
         <v>21</v>
@@ -5084,27 +5138,27 @@
         <v>23</v>
       </c>
       <c r="D105" s="21" t="s">
-        <v>336</v>
+        <v>306</v>
       </c>
       <c r="I105" s="9" t="s">
-        <v>337</v>
+        <v>307</v>
       </c>
       <c r="J105">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="K105" t="s">
-        <v>180</v>
+        <v>283</v>
       </c>
       <c r="L105" t="s">
-        <v>181</v>
+        <v>292</v>
       </c>
       <c r="P105" t="s">
-        <v>338</v>
+        <v>308</v>
       </c>
     </row>
     <row r="106" spans="1:16">
       <c r="A106" t="s">
-        <v>339</v>
+        <v>309</v>
       </c>
       <c r="B106" t="s">
         <v>21</v>
@@ -5113,27 +5167,27 @@
         <v>23</v>
       </c>
       <c r="D106" s="21" t="s">
-        <v>340</v>
+        <v>310</v>
       </c>
       <c r="I106" s="9" t="s">
-        <v>341</v>
+        <v>311</v>
       </c>
       <c r="J106">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="K106" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="L106" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="P106" t="s">
-        <v>342</v>
+        <v>312</v>
       </c>
     </row>
     <row r="107" spans="1:16">
       <c r="A107" t="s">
-        <v>343</v>
+        <v>313</v>
       </c>
       <c r="B107" t="s">
         <v>21</v>
@@ -5142,27 +5196,27 @@
         <v>23</v>
       </c>
       <c r="D107" s="21" t="s">
-        <v>344</v>
+        <v>314</v>
       </c>
       <c r="I107" s="9" t="s">
-        <v>345</v>
+        <v>315</v>
       </c>
       <c r="J107">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K107" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="L107" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="P107" t="s">
-        <v>346</v>
+        <v>316</v>
       </c>
     </row>
     <row r="108" spans="1:16">
       <c r="A108" t="s">
-        <v>347</v>
+        <v>317</v>
       </c>
       <c r="B108" t="s">
         <v>21</v>
@@ -5171,27 +5225,27 @@
         <v>23</v>
       </c>
       <c r="D108" s="21" t="s">
-        <v>348</v>
+        <v>318</v>
       </c>
       <c r="I108" s="9" t="s">
-        <v>349</v>
+        <v>319</v>
       </c>
       <c r="J108">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K108" t="s">
-        <v>309</v>
+        <v>168</v>
       </c>
       <c r="L108" t="s">
-        <v>318</v>
+        <v>169</v>
       </c>
       <c r="P108" t="s">
-        <v>350</v>
+        <v>320</v>
       </c>
     </row>
     <row r="109" spans="1:16">
       <c r="A109" t="s">
-        <v>351</v>
+        <v>321</v>
       </c>
       <c r="B109" t="s">
         <v>21</v>
@@ -5200,27 +5254,27 @@
         <v>23</v>
       </c>
       <c r="D109" s="21" t="s">
-        <v>352</v>
+        <v>322</v>
       </c>
       <c r="I109" s="9" t="s">
-        <v>353</v>
+        <v>323</v>
       </c>
       <c r="J109">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K109" t="s">
-        <v>180</v>
+        <v>283</v>
       </c>
       <c r="L109" t="s">
-        <v>318</v>
+        <v>292</v>
       </c>
       <c r="P109" t="s">
-        <v>354</v>
+        <v>324</v>
       </c>
     </row>
     <row r="110" spans="1:16">
       <c r="A110" t="s">
-        <v>355</v>
+        <v>325</v>
       </c>
       <c r="B110" t="s">
         <v>21</v>
@@ -5229,27 +5283,27 @@
         <v>23</v>
       </c>
       <c r="D110" s="21" t="s">
-        <v>356</v>
+        <v>326</v>
       </c>
       <c r="I110" s="9" t="s">
-        <v>357</v>
+        <v>327</v>
       </c>
       <c r="J110">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="K110" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="L110" t="s">
-        <v>181</v>
+        <v>292</v>
       </c>
       <c r="P110" t="s">
-        <v>358</v>
+        <v>328</v>
       </c>
     </row>
     <row r="111" spans="1:16">
       <c r="A111" t="s">
-        <v>359</v>
+        <v>329</v>
       </c>
       <c r="B111" t="s">
         <v>21</v>
@@ -5258,27 +5312,27 @@
         <v>23</v>
       </c>
       <c r="D111" s="21" t="s">
-        <v>360</v>
+        <v>330</v>
       </c>
       <c r="I111" s="9" t="s">
-        <v>361</v>
+        <v>331</v>
       </c>
       <c r="J111">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="K111" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="L111" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="P111" t="s">
-        <v>362</v>
+        <v>332</v>
       </c>
     </row>
     <row r="112" spans="1:16">
       <c r="A112" t="s">
-        <v>363</v>
+        <v>333</v>
       </c>
       <c r="B112" t="s">
         <v>21</v>
@@ -5287,27 +5341,27 @@
         <v>23</v>
       </c>
       <c r="D112" s="21" t="s">
-        <v>364</v>
+        <v>334</v>
       </c>
       <c r="I112" s="9" t="s">
-        <v>365</v>
+        <v>335</v>
       </c>
       <c r="J112">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K112" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="L112" t="s">
-        <v>309</v>
+        <v>169</v>
       </c>
       <c r="P112" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="113" spans="1:17">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16">
       <c r="A113" t="s">
-        <v>367</v>
+        <v>337</v>
       </c>
       <c r="B113" t="s">
         <v>21</v>
@@ -5316,27 +5370,27 @@
         <v>23</v>
       </c>
       <c r="D113" s="21" t="s">
-        <v>368</v>
+        <v>338</v>
       </c>
       <c r="I113" s="9" t="s">
-        <v>369</v>
+        <v>339</v>
       </c>
       <c r="J113">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="K113" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="L113" t="s">
-        <v>181</v>
+        <v>283</v>
       </c>
       <c r="P113" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="114" spans="1:17">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16">
       <c r="A114" t="s">
-        <v>371</v>
+        <v>341</v>
       </c>
       <c r="B114" t="s">
         <v>21</v>
@@ -5345,27 +5399,27 @@
         <v>23</v>
       </c>
       <c r="D114" s="21" t="s">
-        <v>372</v>
+        <v>342</v>
       </c>
       <c r="I114" s="9" t="s">
-        <v>373</v>
+        <v>343</v>
       </c>
       <c r="J114">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="K114" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="L114" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="P114" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="115" spans="1:17">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16">
       <c r="A115" t="s">
-        <v>375</v>
+        <v>345</v>
       </c>
       <c r="B115" t="s">
         <v>21</v>
@@ -5374,34 +5428,56 @@
         <v>23</v>
       </c>
       <c r="D115" s="21" t="s">
-        <v>376</v>
+        <v>346</v>
       </c>
       <c r="I115" s="9" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
       <c r="J115">
+        <v>37</v>
+      </c>
+      <c r="K115" t="s">
+        <v>169</v>
+      </c>
+      <c r="L115" t="s">
+        <v>168</v>
+      </c>
+      <c r="P115" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16">
+      <c r="A116" t="s">
+        <v>349</v>
+      </c>
+      <c r="B116" t="s">
+        <v>21</v>
+      </c>
+      <c r="C116" t="s">
+        <v>23</v>
+      </c>
+      <c r="D116" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="I116" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="J116">
         <v>40</v>
       </c>
-      <c r="K115" t="s">
-        <v>180</v>
-      </c>
-      <c r="L115" t="s">
-        <v>318</v>
-      </c>
-      <c r="P115" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="116" spans="1:17">
-      <c r="A116" t="s">
-        <v>387</v>
-      </c>
-      <c r="I116" s="9"/>
-      <c r="Q116" s="14"/>
-    </row>
-    <row r="117" spans="1:17">
+      <c r="K116" t="s">
+        <v>168</v>
+      </c>
+      <c r="L116" t="s">
+        <v>292</v>
+      </c>
+      <c r="P116" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16">
       <c r="A117" t="s">
-        <v>379</v>
+        <v>463</v>
       </c>
       <c r="B117" t="s">
         <v>21</v>
@@ -5410,27 +5486,27 @@
         <v>23</v>
       </c>
       <c r="D117" s="21" t="s">
-        <v>380</v>
+        <v>464</v>
       </c>
       <c r="I117" s="9" t="s">
-        <v>381</v>
+        <v>465</v>
       </c>
       <c r="J117">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="K117" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="L117" t="s">
-        <v>318</v>
+        <v>168</v>
       </c>
       <c r="P117" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="118" spans="1:17">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16">
       <c r="A118" t="s">
-        <v>383</v>
+        <v>353</v>
       </c>
       <c r="B118" t="s">
         <v>21</v>
@@ -5439,27 +5515,27 @@
         <v>23</v>
       </c>
       <c r="D118" s="21" t="s">
-        <v>384</v>
+        <v>354</v>
       </c>
       <c r="I118" s="9" t="s">
-        <v>385</v>
+        <v>355</v>
       </c>
       <c r="J118">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="K118" t="s">
-        <v>309</v>
+        <v>169</v>
       </c>
       <c r="L118" t="s">
-        <v>318</v>
+        <v>292</v>
       </c>
       <c r="P118" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="119" spans="1:17">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16">
       <c r="A119" t="s">
-        <v>388</v>
+        <v>357</v>
       </c>
       <c r="B119" t="s">
         <v>21</v>
@@ -5468,27 +5544,27 @@
         <v>23</v>
       </c>
       <c r="D119" s="21" t="s">
-        <v>389</v>
+        <v>358</v>
       </c>
       <c r="I119" s="9" t="s">
-        <v>390</v>
+        <v>359</v>
       </c>
       <c r="J119">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="K119" t="s">
-        <v>309</v>
+        <v>283</v>
       </c>
       <c r="L119" t="s">
-        <v>318</v>
+        <v>292</v>
       </c>
       <c r="P119" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="120" spans="1:17">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16">
       <c r="A120" t="s">
-        <v>392</v>
+        <v>361</v>
       </c>
       <c r="B120" t="s">
         <v>21</v>
@@ -5497,27 +5573,27 @@
         <v>23</v>
       </c>
       <c r="D120" s="21" t="s">
-        <v>393</v>
+        <v>362</v>
       </c>
       <c r="I120" s="9" t="s">
-        <v>394</v>
+        <v>363</v>
       </c>
       <c r="J120">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="K120" t="s">
-        <v>180</v>
+        <v>283</v>
       </c>
       <c r="L120" t="s">
-        <v>181</v>
+        <v>292</v>
       </c>
       <c r="P120" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="121" spans="1:17">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16">
       <c r="A121" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="B121" t="s">
         <v>21</v>
@@ -5525,26 +5601,28 @@
       <c r="C121" t="s">
         <v>23</v>
       </c>
-      <c r="D121" s="21"/>
+      <c r="D121" s="21" t="s">
+        <v>366</v>
+      </c>
       <c r="I121" s="9" t="s">
-        <v>397</v>
+        <v>367</v>
       </c>
       <c r="J121">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K121" t="s">
-        <v>318</v>
+        <v>168</v>
       </c>
       <c r="L121" t="s">
-        <v>309</v>
+        <v>169</v>
       </c>
       <c r="P121" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="122" spans="1:17">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16">
       <c r="A122" t="s">
-        <v>398</v>
+        <v>369</v>
       </c>
       <c r="B122" t="s">
         <v>21</v>
@@ -5552,28 +5630,26 @@
       <c r="C122" t="s">
         <v>23</v>
       </c>
-      <c r="D122" s="21" t="s">
-        <v>399</v>
-      </c>
+      <c r="D122" s="21"/>
       <c r="I122" s="9" t="s">
-        <v>400</v>
+        <v>370</v>
       </c>
       <c r="J122">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K122" t="s">
-        <v>181</v>
+        <v>292</v>
       </c>
       <c r="L122" t="s">
-        <v>318</v>
+        <v>283</v>
       </c>
       <c r="P122" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="123" spans="1:17">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16">
       <c r="A123" t="s">
-        <v>402</v>
+        <v>371</v>
       </c>
       <c r="B123" t="s">
         <v>21</v>
@@ -5581,26 +5657,28 @@
       <c r="C123" t="s">
         <v>23</v>
       </c>
-      <c r="D123" s="21"/>
+      <c r="D123" s="21" t="s">
+        <v>372</v>
+      </c>
       <c r="I123" s="9" t="s">
-        <v>403</v>
+        <v>373</v>
       </c>
       <c r="J123">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K123" t="s">
-        <v>318</v>
+        <v>169</v>
       </c>
       <c r="L123" t="s">
-        <v>181</v>
+        <v>292</v>
       </c>
       <c r="P123" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="124" spans="1:17">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16">
       <c r="A124" t="s">
-        <v>405</v>
+        <v>375</v>
       </c>
       <c r="B124" t="s">
         <v>21</v>
@@ -5608,26 +5686,26 @@
       <c r="C124" t="s">
         <v>23</v>
       </c>
-      <c r="D124" s="9"/>
+      <c r="D124" s="21"/>
       <c r="I124" s="9" t="s">
-        <v>406</v>
+        <v>376</v>
       </c>
       <c r="J124">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="K124" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="L124" t="s">
-        <v>318</v>
-      </c>
-      <c r="P124" s="18" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="125" spans="1:17">
+        <v>169</v>
+      </c>
+      <c r="P124" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16">
       <c r="A125" t="s">
-        <v>408</v>
+        <v>378</v>
       </c>
       <c r="B125" t="s">
         <v>21</v>
@@ -5635,28 +5713,26 @@
       <c r="C125" t="s">
         <v>23</v>
       </c>
-      <c r="D125" s="21" t="s">
-        <v>409</v>
-      </c>
+      <c r="D125" s="9"/>
       <c r="I125" s="9" t="s">
-        <v>410</v>
+        <v>379</v>
       </c>
       <c r="J125">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="K125" t="s">
-        <v>181</v>
+        <v>283</v>
       </c>
       <c r="L125" t="s">
-        <v>309</v>
-      </c>
-      <c r="P125" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="126" spans="1:17">
+        <v>292</v>
+      </c>
+      <c r="P125" s="18" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16">
       <c r="A126" t="s">
-        <v>412</v>
+        <v>381</v>
       </c>
       <c r="B126" t="s">
         <v>21</v>
@@ -5664,26 +5740,28 @@
       <c r="C126" t="s">
         <v>23</v>
       </c>
-      <c r="D126" s="21"/>
+      <c r="D126" s="21" t="s">
+        <v>382</v>
+      </c>
       <c r="I126" s="9" t="s">
-        <v>413</v>
+        <v>383</v>
       </c>
       <c r="J126">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K126" t="s">
-        <v>309</v>
+        <v>169</v>
       </c>
       <c r="L126" t="s">
-        <v>318</v>
+        <v>283</v>
       </c>
       <c r="P126" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="127" spans="1:17">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16">
       <c r="A127" t="s">
-        <v>415</v>
+        <v>385</v>
       </c>
       <c r="B127" t="s">
         <v>21</v>
@@ -5691,28 +5769,26 @@
       <c r="C127" t="s">
         <v>23</v>
       </c>
-      <c r="D127" s="21" t="s">
-        <v>416</v>
-      </c>
+      <c r="D127" s="21"/>
       <c r="I127" s="9" t="s">
-        <v>417</v>
+        <v>386</v>
       </c>
       <c r="J127">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K127" t="s">
-        <v>181</v>
+        <v>283</v>
       </c>
       <c r="L127" t="s">
-        <v>318</v>
+        <v>292</v>
       </c>
       <c r="P127" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="128" spans="1:17">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16">
       <c r="A128" t="s">
-        <v>418</v>
+        <v>388</v>
       </c>
       <c r="B128" t="s">
         <v>21</v>
@@ -5721,27 +5797,27 @@
         <v>23</v>
       </c>
       <c r="D128" s="21" t="s">
-        <v>419</v>
+        <v>389</v>
       </c>
       <c r="I128" s="9" t="s">
-        <v>420</v>
+        <v>390</v>
       </c>
       <c r="J128">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="K128" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="L128" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="P128" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="129" spans="1:16">
       <c r="A129" t="s">
-        <v>421</v>
+        <v>391</v>
       </c>
       <c r="B129" t="s">
         <v>21</v>
@@ -5750,27 +5826,27 @@
         <v>23</v>
       </c>
       <c r="D129" s="21" t="s">
-        <v>422</v>
+        <v>392</v>
       </c>
       <c r="I129" s="9" t="s">
-        <v>423</v>
+        <v>393</v>
       </c>
       <c r="J129">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="K129" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="L129" t="s">
-        <v>318</v>
+        <v>283</v>
       </c>
       <c r="P129" t="s">
-        <v>424</v>
+        <v>170</v>
       </c>
     </row>
     <row r="130" spans="1:16">
       <c r="A130" t="s">
-        <v>425</v>
+        <v>394</v>
       </c>
       <c r="B130" t="s">
         <v>21</v>
@@ -5779,27 +5855,27 @@
         <v>23</v>
       </c>
       <c r="D130" s="21" t="s">
-        <v>426</v>
+        <v>395</v>
       </c>
       <c r="I130" s="9" t="s">
-        <v>427</v>
+        <v>396</v>
       </c>
       <c r="J130">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="K130" t="s">
-        <v>309</v>
+        <v>168</v>
       </c>
       <c r="L130" t="s">
-        <v>181</v>
+        <v>292</v>
       </c>
       <c r="P130" t="s">
-        <v>428</v>
+        <v>397</v>
       </c>
     </row>
     <row r="131" spans="1:16">
       <c r="A131" t="s">
-        <v>429</v>
+        <v>398</v>
       </c>
       <c r="B131" t="s">
         <v>21</v>
@@ -5807,26 +5883,28 @@
       <c r="C131" t="s">
         <v>23</v>
       </c>
-      <c r="D131" s="21"/>
+      <c r="D131" s="21" t="s">
+        <v>399</v>
+      </c>
       <c r="I131" s="9" t="s">
-        <v>430</v>
+        <v>400</v>
       </c>
       <c r="J131">
         <v>35</v>
       </c>
       <c r="K131" t="s">
-        <v>180</v>
+        <v>283</v>
       </c>
       <c r="L131" t="s">
-        <v>318</v>
+        <v>169</v>
       </c>
       <c r="P131" t="s">
-        <v>431</v>
+        <v>401</v>
       </c>
     </row>
     <row r="132" spans="1:16">
       <c r="A132" t="s">
-        <v>432</v>
+        <v>402</v>
       </c>
       <c r="B132" t="s">
         <v>21</v>
@@ -5834,521 +5912,352 @@
       <c r="C132" t="s">
         <v>23</v>
       </c>
-      <c r="D132" s="21" t="s">
-        <v>433</v>
-      </c>
+      <c r="D132" s="21"/>
       <c r="I132" s="9" t="s">
-        <v>434</v>
+        <v>403</v>
       </c>
       <c r="J132">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K132" t="s">
-        <v>309</v>
+        <v>168</v>
       </c>
       <c r="L132" t="s">
-        <v>181</v>
+        <v>292</v>
       </c>
       <c r="P132" t="s">
-        <v>435</v>
+        <v>404</v>
       </c>
     </row>
     <row r="133" spans="1:16">
       <c r="A133" t="s">
-        <v>436</v>
+        <v>405</v>
       </c>
       <c r="B133" t="s">
         <v>21</v>
       </c>
       <c r="C133" t="s">
+        <v>23</v>
+      </c>
+      <c r="D133" s="21" t="s">
+        <v>406</v>
+      </c>
+      <c r="I133" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="J133">
+        <v>37</v>
+      </c>
+      <c r="K133" t="s">
+        <v>283</v>
+      </c>
+      <c r="L133" t="s">
+        <v>169</v>
+      </c>
+      <c r="P133" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16">
+      <c r="A134" t="s">
+        <v>409</v>
+      </c>
+      <c r="B134" t="s">
+        <v>25</v>
+      </c>
+      <c r="C134" t="s">
         <v>22</v>
       </c>
-      <c r="D133" s="21" t="s">
-        <v>437</v>
-      </c>
-      <c r="I133" s="9" t="s">
-        <v>438</v>
-      </c>
-      <c r="J133">
-        <v>43</v>
-      </c>
-      <c r="K133" t="s">
-        <v>181</v>
-      </c>
-      <c r="L133" t="s">
-        <v>309</v>
-      </c>
-      <c r="P133" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="134" spans="1:16">
-      <c r="D134" s="21"/>
-      <c r="I134" s="9"/>
-      <c r="J134">
-        <v>67</v>
-      </c>
-      <c r="K134" t="s">
-        <v>181</v>
-      </c>
-      <c r="L134" t="s">
-        <v>180</v>
+      <c r="D134" s="21" t="s">
+        <v>410</v>
+      </c>
+      <c r="H134" t="s">
+        <v>467</v>
+      </c>
+      <c r="I134" s="9" t="s">
+        <v>426</v>
       </c>
       <c r="P134" t="s">
-        <v>439</v>
+        <v>412</v>
       </c>
     </row>
     <row r="135" spans="1:16">
       <c r="D135" s="21"/>
-      <c r="I135" s="9"/>
-      <c r="J135">
-        <v>91</v>
-      </c>
-      <c r="K135" t="s">
-        <v>180</v>
-      </c>
-      <c r="L135" t="s">
-        <v>181</v>
+      <c r="H135" t="s">
+        <v>470</v>
+      </c>
+      <c r="I135" s="9" t="s">
+        <v>411</v>
       </c>
       <c r="P135" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
     </row>
     <row r="136" spans="1:16">
+      <c r="A136" t="s">
+        <v>413</v>
+      </c>
+      <c r="B136" t="s">
+        <v>25</v>
+      </c>
+      <c r="C136" t="s">
+        <v>22</v>
+      </c>
       <c r="D136" s="21"/>
-      <c r="I136" s="9"/>
-      <c r="J136">
-        <v>126</v>
-      </c>
-      <c r="K136" t="s">
-        <v>309</v>
-      </c>
-      <c r="L136" t="s">
-        <v>318</v>
+      <c r="H136" t="s">
+        <v>468</v>
+      </c>
+      <c r="I136" s="9" t="s">
+        <v>427</v>
       </c>
       <c r="P136" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
     </row>
     <row r="137" spans="1:16">
       <c r="D137" s="21"/>
-      <c r="I137" s="9"/>
-      <c r="J137">
-        <v>143</v>
-      </c>
-      <c r="K137" t="s">
-        <v>309</v>
-      </c>
-      <c r="L137" t="s">
-        <v>181</v>
+      <c r="H137" t="s">
+        <v>469</v>
+      </c>
+      <c r="I137" s="9" t="s">
+        <v>428</v>
       </c>
       <c r="P137" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
     </row>
     <row r="138" spans="1:16">
-      <c r="D138" s="21"/>
-      <c r="I138" s="9"/>
-      <c r="J138">
-        <v>181</v>
-      </c>
-      <c r="K138" t="s">
-        <v>181</v>
-      </c>
-      <c r="L138" t="s">
-        <v>180</v>
+      <c r="A138" t="s">
+        <v>414</v>
+      </c>
+      <c r="B138" t="s">
+        <v>25</v>
+      </c>
+      <c r="C138" t="s">
+        <v>26</v>
+      </c>
+      <c r="D138" s="21" t="s">
+        <v>415</v>
+      </c>
+      <c r="I138" s="9" t="s">
+        <v>461</v>
       </c>
       <c r="P138" t="s">
-        <v>439</v>
+        <v>416</v>
       </c>
     </row>
     <row r="139" spans="1:16">
-      <c r="D139" s="21"/>
-      <c r="I139" s="9"/>
-      <c r="J139">
-        <v>184</v>
-      </c>
-      <c r="K139" t="s">
-        <v>309</v>
-      </c>
-      <c r="L139" t="s">
-        <v>181</v>
+      <c r="A139" t="s">
+        <v>417</v>
+      </c>
+      <c r="B139" t="s">
+        <v>25</v>
+      </c>
+      <c r="C139" t="s">
+        <v>26</v>
+      </c>
+      <c r="D139" s="21" t="s">
+        <v>418</v>
+      </c>
+      <c r="I139" s="9" t="s">
+        <v>462</v>
       </c>
       <c r="P139" t="s">
-        <v>439</v>
+        <v>419</v>
       </c>
     </row>
     <row r="140" spans="1:16">
-      <c r="D140" s="21"/>
-      <c r="I140" s="9"/>
-      <c r="J140">
-        <v>220</v>
-      </c>
-      <c r="K140" t="s">
-        <v>318</v>
-      </c>
-      <c r="L140" t="s">
-        <v>309</v>
+      <c r="A140" t="s">
+        <v>420</v>
+      </c>
+      <c r="B140" t="s">
+        <v>25</v>
+      </c>
+      <c r="C140" t="s">
+        <v>26</v>
+      </c>
+      <c r="D140" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="I140" s="9" t="s">
+        <v>459</v>
       </c>
       <c r="P140" t="s">
-        <v>439</v>
+        <v>422</v>
       </c>
     </row>
     <row r="141" spans="1:16">
-      <c r="D141" s="21"/>
-      <c r="I141" s="9"/>
-      <c r="J141">
-        <v>235</v>
-      </c>
-      <c r="K141" t="s">
-        <v>318</v>
-      </c>
-      <c r="L141" t="s">
-        <v>309</v>
+      <c r="A141" t="s">
+        <v>423</v>
+      </c>
+      <c r="B141" t="s">
+        <v>25</v>
+      </c>
+      <c r="C141" t="s">
+        <v>26</v>
+      </c>
+      <c r="D141" s="21" t="s">
+        <v>424</v>
+      </c>
+      <c r="I141" s="9" t="s">
+        <v>460</v>
       </c>
       <c r="P141" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
     </row>
     <row r="142" spans="1:16">
-      <c r="A142" t="s">
-        <v>440</v>
-      </c>
-      <c r="B142" t="s">
-        <v>21</v>
-      </c>
-      <c r="C142" t="s">
-        <v>22</v>
-      </c>
-      <c r="D142" s="21"/>
-      <c r="I142" s="9" t="s">
-        <v>441</v>
-      </c>
-      <c r="J142">
-        <v>39</v>
-      </c>
-      <c r="K142" t="s">
-        <v>318</v>
-      </c>
-      <c r="L142" t="s">
-        <v>309</v>
-      </c>
-      <c r="P142" t="s">
-        <v>442</v>
-      </c>
+      <c r="I142" s="9"/>
+      <c r="P142" s="12"/>
     </row>
     <row r="143" spans="1:16">
-      <c r="D143" s="21"/>
       <c r="I143" s="9"/>
-      <c r="J143">
-        <v>51</v>
-      </c>
-      <c r="K143" t="s">
-        <v>318</v>
-      </c>
-      <c r="L143" t="s">
-        <v>309</v>
-      </c>
-      <c r="P143" t="s">
-        <v>442</v>
-      </c>
+      <c r="P143" s="12"/>
     </row>
     <row r="144" spans="1:16">
-      <c r="D144" s="21"/>
       <c r="I144" s="9"/>
-      <c r="J144">
-        <v>63</v>
-      </c>
-      <c r="K144" t="s">
-        <v>309</v>
-      </c>
-      <c r="L144" t="s">
-        <v>318</v>
-      </c>
-      <c r="P144" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="145" spans="1:16">
-      <c r="D145" s="21"/>
+      <c r="P144" s="12"/>
+    </row>
+    <row r="145" spans="4:18">
       <c r="I145" s="9"/>
-      <c r="J145">
-        <v>78</v>
-      </c>
-      <c r="K145" t="s">
-        <v>318</v>
-      </c>
-      <c r="L145" t="s">
-        <v>180</v>
-      </c>
-      <c r="P145" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="146" spans="1:16">
-      <c r="D146" s="21"/>
+      <c r="P145" s="12"/>
+    </row>
+    <row r="146" spans="4:18">
+      <c r="D146" s="9"/>
       <c r="I146" s="9"/>
-      <c r="J146">
-        <v>82</v>
-      </c>
-      <c r="K146" t="s">
-        <v>309</v>
-      </c>
-      <c r="L146" t="s">
-        <v>180</v>
-      </c>
-      <c r="P146" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="147" spans="1:16">
-      <c r="D147" s="21"/>
+    </row>
+    <row r="147" spans="4:18">
+      <c r="D147" s="9"/>
       <c r="I147" s="9"/>
-      <c r="J147">
-        <v>147</v>
-      </c>
-      <c r="K147" t="s">
-        <v>181</v>
-      </c>
-      <c r="L147" t="s">
-        <v>180</v>
-      </c>
-      <c r="P147" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="148" spans="1:16">
-      <c r="A148" t="s">
-        <v>443</v>
-      </c>
-      <c r="B148" t="s">
-        <v>20</v>
-      </c>
-      <c r="C148" t="s">
-        <v>26</v>
-      </c>
-      <c r="D148" s="21" t="s">
-        <v>444</v>
-      </c>
-      <c r="I148" s="9" t="s">
-        <v>445</v>
-      </c>
-      <c r="P148" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="149" spans="1:16">
-      <c r="A149" t="s">
-        <v>447</v>
-      </c>
-      <c r="B149" t="s">
-        <v>20</v>
-      </c>
-      <c r="C149" t="s">
-        <v>26</v>
-      </c>
-      <c r="D149" s="21" t="s">
-        <v>448</v>
-      </c>
-      <c r="I149" s="9" t="s">
-        <v>449</v>
-      </c>
-      <c r="P149" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="150" spans="1:16">
-      <c r="A150" t="s">
-        <v>451</v>
-      </c>
-      <c r="B150" t="s">
-        <v>25</v>
-      </c>
-      <c r="C150" t="s">
-        <v>26</v>
-      </c>
-      <c r="D150" s="21" t="s">
-        <v>452</v>
-      </c>
-      <c r="I150" s="9" t="s">
-        <v>453</v>
-      </c>
-      <c r="P150" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="151" spans="1:16">
-      <c r="A151" t="s">
-        <v>455</v>
-      </c>
-      <c r="B151" t="s">
-        <v>25</v>
-      </c>
-      <c r="C151" t="s">
-        <v>26</v>
-      </c>
-      <c r="D151" s="21" t="s">
-        <v>456</v>
-      </c>
-      <c r="I151" s="9" t="s">
-        <v>457</v>
-      </c>
-      <c r="P151" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="152" spans="1:16">
+    </row>
+    <row r="148" spans="4:18">
+      <c r="I148" s="9"/>
+      <c r="P148" s="15"/>
+    </row>
+    <row r="149" spans="4:18">
+      <c r="I149" s="9"/>
+      <c r="P149" s="15"/>
+    </row>
+    <row r="150" spans="4:18">
+      <c r="D150" s="9"/>
+      <c r="I150" s="9"/>
+    </row>
+    <row r="151" spans="4:18">
+      <c r="D151" s="9"/>
+      <c r="I151" s="9"/>
+    </row>
+    <row r="152" spans="4:18">
+      <c r="D152" s="9"/>
       <c r="I152" s="9"/>
-      <c r="P152" s="12"/>
-    </row>
-    <row r="153" spans="1:16">
+    </row>
+    <row r="153" spans="4:18">
+      <c r="D153" s="9"/>
       <c r="I153" s="9"/>
-      <c r="P153" s="12"/>
-    </row>
-    <row r="154" spans="1:16">
+    </row>
+    <row r="154" spans="4:18">
+      <c r="D154" s="9"/>
       <c r="I154" s="9"/>
-      <c r="P154" s="12"/>
-    </row>
-    <row r="155" spans="1:16">
+    </row>
+    <row r="155" spans="4:18">
+      <c r="D155" s="9"/>
       <c r="I155" s="9"/>
-      <c r="P155" s="12"/>
-    </row>
-    <row r="156" spans="1:16">
+      <c r="R155" s="17"/>
+    </row>
+    <row r="156" spans="4:18">
       <c r="D156" s="9"/>
       <c r="I156" s="9"/>
     </row>
-    <row r="157" spans="1:16">
+    <row r="157" spans="4:18">
       <c r="D157" s="9"/>
       <c r="I157" s="9"/>
-    </row>
-    <row r="158" spans="1:16">
+      <c r="P157" s="18"/>
+    </row>
+    <row r="158" spans="4:18">
       <c r="I158" s="9"/>
-      <c r="P158" s="15"/>
-    </row>
-    <row r="159" spans="1:16">
+    </row>
+    <row r="159" spans="4:18">
       <c r="I159" s="9"/>
-      <c r="P159" s="15"/>
-    </row>
-    <row r="160" spans="1:16">
-      <c r="D160" s="9"/>
+    </row>
+    <row r="160" spans="4:18">
       <c r="I160" s="9"/>
     </row>
-    <row r="161" spans="4:18">
-      <c r="D161" s="9"/>
+    <row r="161" spans="1:30">
       <c r="I161" s="9"/>
     </row>
-    <row r="162" spans="4:18">
-      <c r="D162" s="9"/>
+    <row r="162" spans="1:30">
       <c r="I162" s="9"/>
     </row>
-    <row r="163" spans="4:18">
-      <c r="D163" s="9"/>
+    <row r="163" spans="1:30">
       <c r="I163" s="9"/>
     </row>
-    <row r="164" spans="4:18">
-      <c r="D164" s="9"/>
+    <row r="164" spans="1:30">
       <c r="I164" s="9"/>
     </row>
-    <row r="165" spans="4:18">
-      <c r="D165" s="9"/>
+    <row r="165" spans="1:30">
       <c r="I165" s="9"/>
-      <c r="R165" s="17"/>
-    </row>
-    <row r="166" spans="4:18">
-      <c r="D166" s="9"/>
+    </row>
+    <row r="166" spans="1:30">
       <c r="I166" s="9"/>
     </row>
-    <row r="167" spans="4:18">
-      <c r="D167" s="9"/>
+    <row r="167" spans="1:30">
       <c r="I167" s="9"/>
-      <c r="P167" s="18"/>
-    </row>
-    <row r="168" spans="4:18">
+    </row>
+    <row r="168" spans="1:30">
       <c r="I168" s="9"/>
-    </row>
-    <row r="169" spans="4:18">
+      <c r="P168" s="19"/>
+    </row>
+    <row r="169" spans="1:30">
+      <c r="D169" s="9"/>
       <c r="I169" s="9"/>
     </row>
-    <row r="170" spans="4:18">
-      <c r="I170" s="9"/>
-    </row>
-    <row r="171" spans="4:18">
-      <c r="I171" s="9"/>
-    </row>
-    <row r="172" spans="4:18">
+    <row r="170" spans="1:30" s="16" customFormat="1">
+      <c r="A170"/>
+      <c r="B170"/>
+      <c r="C170"/>
+      <c r="D170"/>
+      <c r="E170"/>
+      <c r="F170"/>
+      <c r="G170"/>
+      <c r="H170"/>
+      <c r="I170"/>
+      <c r="J170"/>
+      <c r="K170"/>
+      <c r="L170"/>
+      <c r="M170"/>
+      <c r="N170"/>
+      <c r="O170"/>
+      <c r="P170"/>
+      <c r="Q170" s="1"/>
+      <c r="R170"/>
+      <c r="S170"/>
+      <c r="T170"/>
+      <c r="U170"/>
+      <c r="V170"/>
+      <c r="W170"/>
+      <c r="X170"/>
+      <c r="Y170"/>
+      <c r="Z170"/>
+      <c r="AA170"/>
+      <c r="AB170"/>
+      <c r="AC170"/>
+      <c r="AD170"/>
+    </row>
+    <row r="172" spans="1:30">
       <c r="I172" s="9"/>
-    </row>
-    <row r="173" spans="4:18">
-      <c r="I173" s="9"/>
-    </row>
-    <row r="174" spans="4:18">
-      <c r="I174" s="9"/>
-    </row>
-    <row r="175" spans="4:18">
-      <c r="I175" s="9"/>
-    </row>
-    <row r="176" spans="4:18">
+      <c r="P172" s="18"/>
+    </row>
+    <row r="173" spans="1:30">
+      <c r="D173" s="9"/>
+    </row>
+    <row r="176" spans="1:30">
+      <c r="D176" s="9"/>
       <c r="I176" s="9"/>
     </row>
-    <row r="177" spans="1:30">
+    <row r="177" spans="4:9">
       <c r="I177" s="9"/>
     </row>
-    <row r="178" spans="1:30">
-      <c r="I178" s="9"/>
-      <c r="P178" s="19"/>
-    </row>
-    <row r="179" spans="1:30">
-      <c r="D179" s="9"/>
-      <c r="I179" s="9"/>
-    </row>
-    <row r="180" spans="1:30" s="16" customFormat="1">
-      <c r="A180"/>
-      <c r="B180"/>
-      <c r="C180"/>
-      <c r="D180"/>
-      <c r="E180"/>
-      <c r="F180"/>
-      <c r="G180"/>
-      <c r="H180"/>
-      <c r="I180"/>
-      <c r="J180"/>
-      <c r="K180"/>
-      <c r="L180"/>
-      <c r="M180"/>
-      <c r="N180"/>
-      <c r="O180"/>
-      <c r="P180"/>
-      <c r="Q180" s="1"/>
-      <c r="R180"/>
-      <c r="S180"/>
-      <c r="T180"/>
-      <c r="U180"/>
-      <c r="V180"/>
-      <c r="W180"/>
-      <c r="X180"/>
-      <c r="Y180"/>
-      <c r="Z180"/>
-      <c r="AA180"/>
-      <c r="AB180"/>
-      <c r="AC180"/>
-      <c r="AD180"/>
-    </row>
-    <row r="182" spans="1:30">
-      <c r="I182" s="9"/>
-      <c r="P182" s="18"/>
-    </row>
-    <row r="183" spans="1:30">
-      <c r="D183" s="9"/>
-    </row>
-    <row r="186" spans="1:30">
-      <c r="D186" s="9"/>
-      <c r="I186" s="9"/>
-    </row>
-    <row r="187" spans="1:30">
-      <c r="I187" s="9"/>
-    </row>
-    <row r="188" spans="1:30">
-      <c r="D188" s="9"/>
+    <row r="178" spans="4:9">
+      <c r="D178" s="9"/>
     </row>
   </sheetData>
   <sortState ref="A3:AD178">
@@ -6361,18 +6270,12 @@
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:O1"/>
   </mergeCells>
-  <dataValidations count="10">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B116 B152:B314">
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B11 B13:B22 B24:B27 B30:B37 B40:B55 B92:B304 B89 B57:B87">
       <formula1>$AB$1:$AE$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C116 C152:C314">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C11 C13:C22 C24:C27 C30:C37 C40:C55 C57:C87 C89 C92:C304">
       <formula1>$AB$2:$AE$2</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C11 C13:C22 C24:C27 C30:C37 C40:C55 C57:C86 C88 C91:C115 C117:C151">
-      <formula1>$AC$1:$AC$9</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B11 B13:B22 B24:B27 B30:B37 B40:B55 B57:B86 B88 B91:B115 B117:B151">
-      <formula1>$AB$1:$AB$9</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23 B29">
       <formula1>$AB$1:$AB$4</formula1>
@@ -6386,10 +6289,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28 B38:B39 B56">
       <formula1>$AB$1:$AB$21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87 B89:B90">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B88 B90:B91">
       <formula1>$AB$1:$AB$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C87 C89:C90">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C88 C90:C91">
       <formula1>$AC$1:$AC$10</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fix an incorrect assay in both NGARD and KlebSeq
</commit_message>
<xml_diff>
--- a/assay_data/KlebSeq_assays.xlsx
+++ b/assay_data/KlebSeq_assays.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="3760" yWindow="7380" windowWidth="35280" windowHeight="21360" tabRatio="500"/>
@@ -114,6 +114,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
       <t>/NT</t>
@@ -124,6 +125,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> Sequence</t>
@@ -192,6 +194,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">-lactams, including cephalosporins (e.g., cefalexin) and </t>
@@ -210,6 +213,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (e.g., meropenem or imipenem)</t>
@@ -248,6 +252,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
       <t>-lactams, including cephalosporins (e.g., cefalexin) and</t>
@@ -266,6 +271,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (e.g., meropenem or imipenem)</t>
@@ -327,9 +333,6 @@
   </si>
   <si>
     <t>77-91</t>
-  </si>
-  <si>
-    <t>SAVYD</t>
   </si>
   <si>
     <t>Any</t>
@@ -1331,6 +1334,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
       <t>-lactamase production</t>
@@ -1349,6 +1353,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
       <t>ESBL production</t>
@@ -1375,6 +1380,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
       <t>-lactamase production; carbapenem resistance</t>
@@ -1724,6 +1730,9 @@
   </si>
   <si>
     <t>Positions</t>
+  </si>
+  <si>
+    <t>YAVYD</t>
   </si>
 </sst>
 </file>
@@ -1736,6 +1745,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3073,8 +3083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3173,7 +3183,7 @@
         <v>10</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>12</v>
@@ -3185,10 +3195,10 @@
         <v>14</v>
       </c>
       <c r="N2" s="9" t="s">
+        <v>518</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>519</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>520</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>28</v>
@@ -3200,7 +3210,7 @@
         <v>17</v>
       </c>
       <c r="S2" s="22" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AB2" s="17" t="s">
         <v>21</v>
@@ -3316,7 +3326,7 @@
         <v>44</v>
       </c>
       <c r="S7" s="19" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="8" spans="1:32">
@@ -3339,7 +3349,7 @@
         <v>44</v>
       </c>
       <c r="S8" s="19" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="9" spans="1:32">
@@ -3362,7 +3372,7 @@
         <v>50</v>
       </c>
       <c r="S9" s="19" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="10" spans="1:32">
@@ -3385,7 +3395,7 @@
         <v>50</v>
       </c>
       <c r="S10" s="19" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="11" spans="1:32">
@@ -3399,7 +3409,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>54</v>
@@ -3408,7 +3418,7 @@
         <v>55</v>
       </c>
       <c r="S11" s="20" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="12" spans="1:32">
@@ -3422,7 +3432,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>57</v>
@@ -3431,7 +3441,7 @@
         <v>55</v>
       </c>
       <c r="S12" s="20" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="13" spans="1:32">
@@ -3445,7 +3455,7 @@
         <v>25</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>59</v>
@@ -3455,7 +3465,7 @@
         <v>55</v>
       </c>
       <c r="S13" s="20" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="14" spans="1:32">
@@ -3469,7 +3479,7 @@
         <v>25</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>61</v>
@@ -3479,7 +3489,7 @@
         <v>55</v>
       </c>
       <c r="S14" s="20" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="15" spans="1:32">
@@ -3503,7 +3513,7 @@
         <v>55</v>
       </c>
       <c r="S15" s="20" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="16" spans="1:32">
@@ -3527,7 +3537,7 @@
         <v>55</v>
       </c>
       <c r="S16" s="20" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -3541,7 +3551,7 @@
         <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G17" t="s">
         <v>67</v>
@@ -3553,21 +3563,21 @@
         <v>69</v>
       </c>
       <c r="P17" t="s">
+        <v>520</v>
+      </c>
+      <c r="Q17" t="s">
         <v>70</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>71</v>
       </c>
-      <c r="R17" t="s">
-        <v>72</v>
-      </c>
       <c r="S17" s="19" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
@@ -3576,30 +3586,30 @@
         <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I18" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="O18" t="s">
         <v>74</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>75</v>
       </c>
-      <c r="P18" t="s">
-        <v>76</v>
-      </c>
       <c r="Q18" t="s">
+        <v>70</v>
+      </c>
+      <c r="R18" t="s">
         <v>71</v>
       </c>
-      <c r="R18" t="s">
-        <v>72</v>
-      </c>
       <c r="S18" s="19" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -3608,21 +3618,21 @@
         <v>25</v>
       </c>
       <c r="D19" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="R19" t="s">
         <v>79</v>
       </c>
-      <c r="R19" t="s">
-        <v>80</v>
-      </c>
       <c r="S19" s="19" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
@@ -3631,21 +3641,21 @@
         <v>25</v>
       </c>
       <c r="D20" t="s">
+        <v>81</v>
+      </c>
+      <c r="I20" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="I20" s="8" t="s">
-        <v>83</v>
-      </c>
       <c r="R20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S20" s="19" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -3654,21 +3664,21 @@
         <v>25</v>
       </c>
       <c r="D21" t="s">
+        <v>84</v>
+      </c>
+      <c r="I21" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>86</v>
-      </c>
       <c r="R21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S21" s="19" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="22" spans="1:19">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
@@ -3677,21 +3687,21 @@
         <v>25</v>
       </c>
       <c r="D22" t="s">
+        <v>87</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="I22" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="R22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S22" s="19" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -3700,21 +3710,21 @@
         <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="R23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S23" s="19" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="24" spans="1:19">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
@@ -3723,21 +3733,21 @@
         <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="R24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S24" s="19" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
@@ -3746,21 +3756,21 @@
         <v>25</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="R25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S25" s="19" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="26" spans="1:19">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B26" t="s">
         <v>19</v>
@@ -3769,21 +3779,21 @@
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S26" s="19" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
         <v>19</v>
@@ -3792,21 +3802,21 @@
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S27" s="19" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="28" spans="1:19">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" t="s">
         <v>24</v>
@@ -3815,21 +3825,21 @@
         <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="R28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S28" s="19" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="29" spans="1:19">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B29" t="s">
         <v>24</v>
@@ -3838,21 +3848,21 @@
         <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="R29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S29" s="19" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="30" spans="1:19">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B30" t="s">
         <v>24</v>
@@ -3861,21 +3871,21 @@
         <v>25</v>
       </c>
       <c r="D30" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="R30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S30" s="19" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="31" spans="1:19">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
         <v>24</v>
@@ -3884,21 +3894,21 @@
         <v>25</v>
       </c>
       <c r="D31" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="R31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S31" s="19" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="32" spans="1:19">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B32" t="s">
         <v>19</v>
@@ -3907,21 +3917,21 @@
         <v>25</v>
       </c>
       <c r="D32" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S32" s="19" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="33" spans="1:19">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B33" t="s">
         <v>19</v>
@@ -3930,21 +3940,21 @@
         <v>25</v>
       </c>
       <c r="D33" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="R33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S33" s="19" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="34" spans="1:19">
       <c r="A34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B34" t="s">
         <v>19</v>
@@ -3953,21 +3963,21 @@
         <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I34" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="R34" t="s">
         <v>107</v>
       </c>
-      <c r="R34" t="s">
-        <v>108</v>
-      </c>
       <c r="S34" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="35" spans="1:19">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B35" t="s">
         <v>19</v>
@@ -3976,21 +3986,21 @@
         <v>25</v>
       </c>
       <c r="D35" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S35" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="36" spans="1:19">
       <c r="A36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B36" t="s">
         <v>19</v>
@@ -3999,21 +4009,21 @@
         <v>25</v>
       </c>
       <c r="D36" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S36" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="37" spans="1:19">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B37" t="s">
         <v>24</v>
@@ -4022,21 +4032,21 @@
         <v>25</v>
       </c>
       <c r="D37" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="R37" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S37" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="38" spans="1:19">
       <c r="A38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B38" t="s">
         <v>24</v>
@@ -4045,21 +4055,21 @@
         <v>25</v>
       </c>
       <c r="D38" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="R38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S38" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="39" spans="1:19">
       <c r="A39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B39" t="s">
         <v>24</v>
@@ -4068,21 +4078,21 @@
         <v>25</v>
       </c>
       <c r="D39" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="R39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S39" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B40" t="s">
         <v>19</v>
@@ -4091,21 +4101,21 @@
         <v>25</v>
       </c>
       <c r="D40" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="R40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S40" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="41" spans="1:19">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B41" t="s">
         <v>19</v>
@@ -4114,21 +4124,21 @@
         <v>25</v>
       </c>
       <c r="D41" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S41" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="42" spans="1:19">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B42" t="s">
         <v>19</v>
@@ -4137,21 +4147,21 @@
         <v>25</v>
       </c>
       <c r="D42" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="R42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S42" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="43" spans="1:19">
       <c r="A43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B43" t="s">
         <v>19</v>
@@ -4160,21 +4170,21 @@
         <v>25</v>
       </c>
       <c r="D43" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S43" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="44" spans="1:19">
       <c r="A44" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B44" t="s">
         <v>19</v>
@@ -4183,21 +4193,21 @@
         <v>25</v>
       </c>
       <c r="D44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S44" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B45" t="s">
         <v>19</v>
@@ -4206,21 +4216,21 @@
         <v>25</v>
       </c>
       <c r="D45" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S45" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="46" spans="1:19">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B46" t="s">
         <v>19</v>
@@ -4229,21 +4239,21 @@
         <v>25</v>
       </c>
       <c r="D46" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S46" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="47" spans="1:19">
       <c r="A47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B47" t="s">
         <v>19</v>
@@ -4252,21 +4262,21 @@
         <v>25</v>
       </c>
       <c r="D47" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S47" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B48" t="s">
         <v>19</v>
@@ -4275,21 +4285,21 @@
         <v>25</v>
       </c>
       <c r="D48" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S48" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="49" spans="1:19">
       <c r="A49" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B49" t="s">
         <v>19</v>
@@ -4298,21 +4308,21 @@
         <v>25</v>
       </c>
       <c r="D49" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="R49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S49" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="50" spans="1:19">
       <c r="A50" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B50" t="s">
         <v>19</v>
@@ -4321,21 +4331,21 @@
         <v>25</v>
       </c>
       <c r="D50" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S50" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="51" spans="1:19">
       <c r="A51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B51" t="s">
         <v>19</v>
@@ -4344,21 +4354,21 @@
         <v>25</v>
       </c>
       <c r="D51" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S51" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="52" spans="1:19">
       <c r="A52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B52" t="s">
         <v>19</v>
@@ -4367,21 +4377,21 @@
         <v>25</v>
       </c>
       <c r="D52" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S52" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="53" spans="1:19">
       <c r="A53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B53" t="s">
         <v>19</v>
@@ -4390,21 +4400,21 @@
         <v>25</v>
       </c>
       <c r="D53" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S53" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="54" spans="1:19">
       <c r="A54" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B54" t="s">
         <v>19</v>
@@ -4413,21 +4423,21 @@
         <v>25</v>
       </c>
       <c r="D54" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S54" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="55" spans="1:19">
       <c r="A55" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B55" t="s">
         <v>24</v>
@@ -4436,21 +4446,21 @@
         <v>25</v>
       </c>
       <c r="D55" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="R55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S55" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="56" spans="1:19">
       <c r="A56" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B56" t="s">
         <v>24</v>
@@ -4459,21 +4469,21 @@
         <v>25</v>
       </c>
       <c r="D56" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="R56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S56" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="57" spans="1:19">
       <c r="A57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B57" t="s">
         <v>24</v>
@@ -4482,21 +4492,21 @@
         <v>25</v>
       </c>
       <c r="D57" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="R57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S57" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="58" spans="1:19">
       <c r="A58" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B58" t="s">
         <v>19</v>
@@ -4505,21 +4515,21 @@
         <v>25</v>
       </c>
       <c r="D58" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S58" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="59" spans="1:19">
       <c r="A59" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
         <v>19</v>
@@ -4528,21 +4538,21 @@
         <v>25</v>
       </c>
       <c r="D59" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R59" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S59" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="60" spans="1:19">
       <c r="A60" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B60" t="s">
         <v>19</v>
@@ -4551,21 +4561,21 @@
         <v>25</v>
       </c>
       <c r="D60" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R60" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S60" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="61" spans="1:19">
       <c r="A61" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B61" t="s">
         <v>19</v>
@@ -4574,21 +4584,21 @@
         <v>25</v>
       </c>
       <c r="D61" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I61" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R61" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S61" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="62" spans="1:19">
       <c r="A62" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B62" t="s">
         <v>20</v>
@@ -4597,28 +4607,28 @@
         <v>22</v>
       </c>
       <c r="D62" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I62" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="I62" s="8" t="s">
-        <v>159</v>
       </c>
       <c r="K62" s="18">
         <v>35</v>
       </c>
       <c r="L62" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="M62" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="M62" s="18" t="s">
+      <c r="R62" s="15" t="s">
         <v>161</v>
-      </c>
-      <c r="R62" s="15" t="s">
-        <v>162</v>
       </c>
       <c r="S62" s="19"/>
     </row>
     <row r="63" spans="1:19">
       <c r="A63" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B63" t="s">
         <v>24</v>
@@ -4627,19 +4637,19 @@
         <v>22</v>
       </c>
       <c r="D63" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="I63" t="s">
         <v>164</v>
       </c>
-      <c r="I63" t="s">
+      <c r="R63" t="s">
         <v>165</v>
-      </c>
-      <c r="R63" t="s">
-        <v>166</v>
       </c>
       <c r="S63" s="19"/>
     </row>
     <row r="64" spans="1:19">
       <c r="A64" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B64" t="s">
         <v>19</v>
@@ -4648,19 +4658,19 @@
         <v>27</v>
       </c>
       <c r="D64" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="I64" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="I64" s="8" t="s">
+      <c r="R64" t="s">
         <v>169</v>
-      </c>
-      <c r="R64" t="s">
-        <v>170</v>
       </c>
       <c r="S64" s="19"/>
     </row>
     <row r="65" spans="1:31">
       <c r="A65" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B65" t="s">
         <v>19</v>
@@ -4669,19 +4679,19 @@
         <v>27</v>
       </c>
       <c r="D65" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="I65" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I65" s="8" t="s">
-        <v>173</v>
-      </c>
       <c r="R65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="S65" s="19"/>
     </row>
     <row r="66" spans="1:31">
       <c r="A66" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B66" t="s">
         <v>19</v>
@@ -4690,19 +4700,19 @@
         <v>27</v>
       </c>
       <c r="D66" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="I66" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="I66" s="8" t="s">
-        <v>176</v>
-      </c>
       <c r="R66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="S66" s="19"/>
     </row>
     <row r="67" spans="1:31">
       <c r="A67" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B67" t="s">
         <v>19</v>
@@ -4711,19 +4721,19 @@
         <v>27</v>
       </c>
       <c r="D67" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="I67" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="I67" s="8" t="s">
-        <v>179</v>
-      </c>
       <c r="R67" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="S67" s="19"/>
     </row>
     <row r="68" spans="1:31">
       <c r="A68" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B68" t="s">
         <v>19</v>
@@ -4732,19 +4742,19 @@
         <v>27</v>
       </c>
       <c r="D68" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="I68" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="I68" s="8" t="s">
+      <c r="R68" t="s">
         <v>182</v>
-      </c>
-      <c r="R68" t="s">
-        <v>183</v>
       </c>
       <c r="S68" s="19"/>
     </row>
     <row r="69" spans="1:31">
       <c r="A69" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B69" t="s">
         <v>19</v>
@@ -4753,19 +4763,19 @@
         <v>27</v>
       </c>
       <c r="D69" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="I69" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="I69" s="8" t="s">
+      <c r="R69" t="s">
         <v>186</v>
-      </c>
-      <c r="R69" t="s">
-        <v>187</v>
       </c>
       <c r="S69" s="19"/>
     </row>
     <row r="70" spans="1:31">
       <c r="A70" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B70" t="s">
         <v>19</v>
@@ -4774,19 +4784,19 @@
         <v>27</v>
       </c>
       <c r="D70" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="I70" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="I70" s="8" t="s">
-        <v>190</v>
-      </c>
       <c r="R70" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="S70" s="19"/>
     </row>
     <row r="71" spans="1:31">
       <c r="A71" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B71" t="s">
         <v>19</v>
@@ -4795,19 +4805,19 @@
         <v>27</v>
       </c>
       <c r="D71" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="I71" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="I71" s="8" t="s">
-        <v>193</v>
-      </c>
       <c r="R71" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="S71" s="19"/>
     </row>
     <row r="72" spans="1:31">
       <c r="A72" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B72" t="s">
         <v>19</v>
@@ -4816,19 +4826,19 @@
         <v>27</v>
       </c>
       <c r="D72" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="I72" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="I72" s="8" t="s">
-        <v>196</v>
-      </c>
       <c r="R72" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="S72" s="19"/>
     </row>
     <row r="73" spans="1:31">
       <c r="A73" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B73" t="s">
         <v>19</v>
@@ -4837,19 +4847,19 @@
         <v>27</v>
       </c>
       <c r="D73" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="I73" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="I73" s="8" t="s">
+      <c r="R73" t="s">
         <v>199</v>
-      </c>
-      <c r="R73" t="s">
-        <v>200</v>
       </c>
       <c r="S73" s="19"/>
     </row>
     <row r="74" spans="1:31">
       <c r="A74" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B74" t="s">
         <v>19</v>
@@ -4858,19 +4868,19 @@
         <v>27</v>
       </c>
       <c r="D74" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="I74" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="I74" s="8" t="s">
-        <v>203</v>
-      </c>
       <c r="R74" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="S74" s="19"/>
     </row>
     <row r="75" spans="1:31">
       <c r="A75" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B75" t="s">
         <v>19</v>
@@ -4879,19 +4889,19 @@
         <v>27</v>
       </c>
       <c r="D75" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="I75" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="I75" s="8" t="s">
+      <c r="R75" t="s">
         <v>206</v>
-      </c>
-      <c r="R75" t="s">
-        <v>207</v>
       </c>
       <c r="S75" s="19"/>
     </row>
     <row r="76" spans="1:31">
       <c r="A76" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B76" t="s">
         <v>19</v>
@@ -4900,19 +4910,19 @@
         <v>27</v>
       </c>
       <c r="D76" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="I76" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="I76" s="8" t="s">
+      <c r="R76" t="s">
         <v>210</v>
-      </c>
-      <c r="R76" t="s">
-        <v>211</v>
       </c>
       <c r="S76" s="19"/>
     </row>
     <row r="77" spans="1:31">
       <c r="A77" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B77" t="s">
         <v>19</v>
@@ -4921,19 +4931,19 @@
         <v>27</v>
       </c>
       <c r="D77" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="I77" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="I77" s="8" t="s">
+      <c r="R77" t="s">
         <v>214</v>
-      </c>
-      <c r="R77" t="s">
-        <v>215</v>
       </c>
       <c r="S77" s="19"/>
     </row>
     <row r="78" spans="1:31">
       <c r="A78" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B78" t="s">
         <v>24</v>
@@ -4942,21 +4952,21 @@
         <v>25</v>
       </c>
       <c r="D78" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I78" s="8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="R78" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="S78" s="19" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="79" spans="1:31">
       <c r="A79" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B79" t="s">
         <v>24</v>
@@ -4965,16 +4975,16 @@
         <v>25</v>
       </c>
       <c r="D79" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I79" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="R79" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S79" s="19" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="AD79" s="17" t="s">
         <v>26</v>
@@ -4985,7 +4995,7 @@
     </row>
     <row r="80" spans="1:31">
       <c r="A80" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B80" t="s">
         <v>19</v>
@@ -4994,21 +5004,21 @@
         <v>25</v>
       </c>
       <c r="D80" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I80" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="R80" t="s">
         <v>221</v>
       </c>
-      <c r="R80" t="s">
-        <v>222</v>
-      </c>
       <c r="S80" s="19" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="81" spans="1:19">
       <c r="A81" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B81" t="s">
         <v>24</v>
@@ -5017,21 +5027,21 @@
         <v>25</v>
       </c>
       <c r="D81" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I81" s="8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="R81" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="S81" s="19" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="82" spans="1:19">
       <c r="A82" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B82" t="s">
         <v>24</v>
@@ -5040,21 +5050,21 @@
         <v>25</v>
       </c>
       <c r="D82" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I82" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="R82" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S82" s="19" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="83" spans="1:19">
       <c r="A83" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B83" t="s">
         <v>24</v>
@@ -5063,39 +5073,39 @@
         <v>25</v>
       </c>
       <c r="D83" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H83" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="I83" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="R83" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S83" s="19" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="84" spans="1:19">
       <c r="D84" s="18"/>
       <c r="H84" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I84" s="8" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="R84" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S84" s="19" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="85" spans="1:19">
       <c r="A85" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B85" t="s">
         <v>19</v>
@@ -5104,21 +5114,21 @@
         <v>25</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I85" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="R85" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S85" s="19" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="86" spans="1:19">
       <c r="A86" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B86" t="s">
         <v>24</v>
@@ -5127,21 +5137,21 @@
         <v>25</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I86" s="8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="R86" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="S86" s="19" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="87" spans="1:19">
       <c r="A87" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B87" t="s">
         <v>24</v>
@@ -5150,21 +5160,21 @@
         <v>25</v>
       </c>
       <c r="D87" s="18" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="R87" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="S87" s="19" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="88" spans="1:19">
       <c r="A88" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B88" t="s">
         <v>24</v>
@@ -5173,21 +5183,21 @@
         <v>25</v>
       </c>
       <c r="D88" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="R88" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="S88" s="19" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="89" spans="1:19">
       <c r="A89" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B89" t="s">
         <v>19</v>
@@ -5196,21 +5206,21 @@
         <v>25</v>
       </c>
       <c r="D89" s="18" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I89" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="R89" t="s">
         <v>237</v>
       </c>
-      <c r="R89" t="s">
-        <v>238</v>
-      </c>
       <c r="S89" s="19" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="90" spans="1:19">
       <c r="A90" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B90" t="s">
         <v>24</v>
@@ -5219,21 +5229,21 @@
         <v>25</v>
       </c>
       <c r="D90" s="18" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I90" s="8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="R90" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="S90" s="19" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="91" spans="1:19">
       <c r="A91" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B91" t="s">
         <v>24</v>
@@ -5242,21 +5252,21 @@
         <v>25</v>
       </c>
       <c r="D91" s="18" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I91" s="8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="R91" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="S91" s="19" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="92" spans="1:19">
       <c r="A92" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B92" t="s">
         <v>19</v>
@@ -5265,21 +5275,21 @@
         <v>25</v>
       </c>
       <c r="D92" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="I92" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="I92" s="8" t="s">
+      <c r="R92" t="s">
         <v>244</v>
       </c>
-      <c r="R92" t="s">
-        <v>245</v>
-      </c>
       <c r="S92" s="19" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="93" spans="1:19">
       <c r="A93" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B93" t="s">
         <v>24</v>
@@ -5288,21 +5298,21 @@
         <v>25</v>
       </c>
       <c r="D93" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="I93" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="R93" t="s">
         <v>247</v>
       </c>
-      <c r="I93" s="8" t="s">
-        <v>438</v>
-      </c>
-      <c r="R93" t="s">
-        <v>248</v>
-      </c>
       <c r="S93" s="19" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="94" spans="1:19">
       <c r="A94" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B94" t="s">
         <v>24</v>
@@ -5311,21 +5321,21 @@
         <v>25</v>
       </c>
       <c r="D94" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I94" s="8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="R94" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="S94" s="19" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="95" spans="1:19">
       <c r="A95" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B95" t="s">
         <v>24</v>
@@ -5334,21 +5344,21 @@
         <v>25</v>
       </c>
       <c r="D95" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I95" s="8" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="R95" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="S95" s="19" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="96" spans="1:19">
       <c r="A96" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B96" t="s">
         <v>24</v>
@@ -5357,21 +5367,21 @@
         <v>25</v>
       </c>
       <c r="D96" s="18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I96" s="8" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="R96" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="S96" s="19" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="97" spans="1:19">
       <c r="A97" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B97" t="s">
         <v>20</v>
@@ -5380,28 +5390,28 @@
         <v>22</v>
       </c>
       <c r="D97" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="I97" s="8" t="s">
         <v>256</v>
-      </c>
-      <c r="I97" s="8" t="s">
-        <v>257</v>
       </c>
       <c r="K97" s="18">
         <v>34</v>
       </c>
       <c r="L97" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="M97" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="M97" s="18" t="s">
-        <v>161</v>
-      </c>
       <c r="R97" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="S97" s="19"/>
     </row>
     <row r="98" spans="1:19">
       <c r="A98" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B98" t="s">
         <v>20</v>
@@ -5410,28 +5420,28 @@
         <v>22</v>
       </c>
       <c r="D98" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="I98" s="8" t="s">
         <v>260</v>
-      </c>
-      <c r="I98" s="8" t="s">
-        <v>261</v>
       </c>
       <c r="K98" s="18">
         <v>34</v>
       </c>
       <c r="L98" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="M98" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="M98" s="18" t="s">
-        <v>161</v>
-      </c>
       <c r="R98" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="S98" s="19"/>
     </row>
     <row r="99" spans="1:19">
       <c r="A99" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B99" t="s">
         <v>20</v>
@@ -5440,28 +5450,28 @@
         <v>22</v>
       </c>
       <c r="D99" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="I99" s="8" t="s">
         <v>264</v>
-      </c>
-      <c r="I99" s="8" t="s">
-        <v>265</v>
       </c>
       <c r="K99" s="18">
         <v>34</v>
       </c>
       <c r="L99" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="M99" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="R99" t="s">
         <v>266</v>
-      </c>
-      <c r="M99" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="R99" t="s">
-        <v>267</v>
       </c>
       <c r="S99" s="19"/>
     </row>
     <row r="100" spans="1:19">
       <c r="A100" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B100" t="s">
         <v>20</v>
@@ -5470,28 +5480,28 @@
         <v>22</v>
       </c>
       <c r="D100" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="I100" s="8" t="s">
         <v>269</v>
-      </c>
-      <c r="I100" s="8" t="s">
-        <v>270</v>
       </c>
       <c r="K100" s="18">
         <v>40</v>
       </c>
       <c r="L100" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="M100" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="M100" s="18" t="s">
-        <v>161</v>
-      </c>
       <c r="R100" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="S100" s="19"/>
     </row>
     <row r="101" spans="1:19">
       <c r="A101" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B101" t="s">
         <v>20</v>
@@ -5500,28 +5510,28 @@
         <v>22</v>
       </c>
       <c r="D101" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="I101" s="8" t="s">
         <v>273</v>
-      </c>
-      <c r="I101" s="8" t="s">
-        <v>274</v>
       </c>
       <c r="K101" s="18">
         <v>35</v>
       </c>
       <c r="L101" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M101" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="R101" t="s">
         <v>275</v>
-      </c>
-      <c r="R101" t="s">
-        <v>276</v>
       </c>
       <c r="S101" s="19"/>
     </row>
     <row r="102" spans="1:19">
       <c r="A102" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B102" t="s">
         <v>20</v>
@@ -5530,28 +5540,28 @@
         <v>22</v>
       </c>
       <c r="D102" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="I102" s="8" t="s">
         <v>278</v>
-      </c>
-      <c r="I102" s="8" t="s">
-        <v>279</v>
       </c>
       <c r="K102" s="18">
         <v>26</v>
       </c>
       <c r="L102" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="M102" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="M102" s="18" t="s">
-        <v>161</v>
-      </c>
       <c r="R102" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="S102" s="19"/>
     </row>
     <row r="103" spans="1:19">
       <c r="A103" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B103" t="s">
         <v>20</v>
@@ -5560,28 +5570,28 @@
         <v>22</v>
       </c>
       <c r="D103" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I103" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="K103" s="18">
+        <v>25</v>
+      </c>
+      <c r="L103" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="M103" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="R103" t="s">
         <v>282</v>
-      </c>
-      <c r="K103" s="18">
-        <v>25</v>
-      </c>
-      <c r="L103" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="M103" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="R103" t="s">
-        <v>283</v>
       </c>
       <c r="S103" s="19"/>
     </row>
     <row r="104" spans="1:19">
       <c r="A104" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B104" t="s">
         <v>20</v>
@@ -5590,28 +5600,28 @@
         <v>22</v>
       </c>
       <c r="D104" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="I104" s="8" t="s">
         <v>285</v>
-      </c>
-      <c r="I104" s="8" t="s">
-        <v>286</v>
       </c>
       <c r="K104" s="18">
         <v>37</v>
       </c>
       <c r="L104" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M104" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R104" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S104" s="19"/>
     </row>
     <row r="105" spans="1:19">
       <c r="A105" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B105" t="s">
         <v>20</v>
@@ -5620,28 +5630,28 @@
         <v>22</v>
       </c>
       <c r="D105" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="I105" s="8" t="s">
         <v>289</v>
-      </c>
-      <c r="I105" s="8" t="s">
-        <v>290</v>
       </c>
       <c r="K105" s="18">
         <v>31</v>
       </c>
       <c r="L105" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M105" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R105" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="S105" s="19"/>
     </row>
     <row r="106" spans="1:19">
       <c r="A106" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B106" t="s">
         <v>20</v>
@@ -5650,28 +5660,28 @@
         <v>22</v>
       </c>
       <c r="D106" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="I106" s="8" t="s">
         <v>293</v>
-      </c>
-      <c r="I106" s="8" t="s">
-        <v>294</v>
       </c>
       <c r="K106" s="18">
         <v>41</v>
       </c>
       <c r="L106" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="M106" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="M106" s="18" t="s">
-        <v>161</v>
-      </c>
       <c r="R106" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="S106" s="19"/>
     </row>
     <row r="107" spans="1:19">
       <c r="A107" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B107" t="s">
         <v>20</v>
@@ -5680,28 +5690,28 @@
         <v>22</v>
       </c>
       <c r="D107" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="I107" s="8" t="s">
         <v>297</v>
-      </c>
-      <c r="I107" s="8" t="s">
-        <v>298</v>
       </c>
       <c r="K107" s="18">
         <v>27</v>
       </c>
       <c r="L107" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="M107" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="M107" s="18" t="s">
-        <v>161</v>
-      </c>
       <c r="R107" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="S107" s="19"/>
     </row>
     <row r="108" spans="1:19">
       <c r="A108" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B108" t="s">
         <v>20</v>
@@ -5710,28 +5720,28 @@
         <v>22</v>
       </c>
       <c r="D108" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="I108" s="8" t="s">
         <v>301</v>
-      </c>
-      <c r="I108" s="8" t="s">
-        <v>302</v>
       </c>
       <c r="K108" s="18">
         <v>31</v>
       </c>
       <c r="L108" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="M108" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="M108" s="18" t="s">
-        <v>161</v>
-      </c>
       <c r="R108" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="S108" s="19"/>
     </row>
     <row r="109" spans="1:19">
       <c r="A109" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B109" t="s">
         <v>20</v>
@@ -5740,28 +5750,28 @@
         <v>22</v>
       </c>
       <c r="D109" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="I109" s="8" t="s">
         <v>305</v>
-      </c>
-      <c r="I109" s="8" t="s">
-        <v>306</v>
       </c>
       <c r="K109" s="18">
         <v>29</v>
       </c>
       <c r="L109" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M109" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R109" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="S109" s="19"/>
     </row>
     <row r="110" spans="1:19">
       <c r="A110" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B110" t="s">
         <v>20</v>
@@ -5770,28 +5780,28 @@
         <v>22</v>
       </c>
       <c r="D110" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="I110" s="8" t="s">
         <v>309</v>
-      </c>
-      <c r="I110" s="8" t="s">
-        <v>310</v>
       </c>
       <c r="K110" s="18">
         <v>27</v>
       </c>
       <c r="L110" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M110" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R110" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="S110" s="19"/>
     </row>
     <row r="111" spans="1:19">
       <c r="A111" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B111" t="s">
         <v>20</v>
@@ -5800,28 +5810,28 @@
         <v>22</v>
       </c>
       <c r="D111" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="I111" s="8" t="s">
         <v>313</v>
-      </c>
-      <c r="I111" s="8" t="s">
-        <v>314</v>
       </c>
       <c r="K111" s="18">
         <v>41</v>
       </c>
       <c r="L111" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="M111" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="M111" s="18" t="s">
-        <v>161</v>
-      </c>
       <c r="R111" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="S111" s="19"/>
     </row>
     <row r="112" spans="1:19">
       <c r="A112" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B112" t="s">
         <v>20</v>
@@ -5830,28 +5840,28 @@
         <v>22</v>
       </c>
       <c r="D112" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="I112" s="8" t="s">
         <v>317</v>
-      </c>
-      <c r="I112" s="8" t="s">
-        <v>318</v>
       </c>
       <c r="K112" s="18">
         <v>34</v>
       </c>
       <c r="L112" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="M112" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="M112" s="18" t="s">
-        <v>161</v>
-      </c>
       <c r="R112" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="S112" s="19"/>
     </row>
     <row r="113" spans="1:19">
       <c r="A113" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B113" t="s">
         <v>20</v>
@@ -5860,28 +5870,28 @@
         <v>22</v>
       </c>
       <c r="D113" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="I113" s="8" t="s">
         <v>321</v>
-      </c>
-      <c r="I113" s="8" t="s">
-        <v>322</v>
       </c>
       <c r="K113" s="18">
         <v>30</v>
       </c>
       <c r="L113" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M113" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="R113" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="S113" s="19"/>
     </row>
     <row r="114" spans="1:19">
       <c r="A114" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B114" t="s">
         <v>20</v>
@@ -5890,28 +5900,28 @@
         <v>22</v>
       </c>
       <c r="D114" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="I114" s="8" t="s">
         <v>325</v>
-      </c>
-      <c r="I114" s="8" t="s">
-        <v>326</v>
       </c>
       <c r="K114" s="18">
         <v>57</v>
       </c>
       <c r="L114" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="M114" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="M114" s="18" t="s">
-        <v>161</v>
-      </c>
       <c r="R114" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S114" s="19"/>
     </row>
     <row r="115" spans="1:19">
       <c r="A115" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B115" t="s">
         <v>20</v>
@@ -5920,28 +5930,28 @@
         <v>22</v>
       </c>
       <c r="D115" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="I115" s="8" t="s">
         <v>329</v>
-      </c>
-      <c r="I115" s="8" t="s">
-        <v>330</v>
       </c>
       <c r="K115" s="18">
         <v>37</v>
       </c>
       <c r="L115" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M115" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R115" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="S115" s="19"/>
     </row>
     <row r="116" spans="1:19">
       <c r="A116" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B116" t="s">
         <v>20</v>
@@ -5950,28 +5960,28 @@
         <v>22</v>
       </c>
       <c r="D116" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="I116" s="8" t="s">
         <v>333</v>
-      </c>
-      <c r="I116" s="8" t="s">
-        <v>334</v>
       </c>
       <c r="K116" s="18">
         <v>40</v>
       </c>
       <c r="L116" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M116" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R116" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="S116" s="19"/>
     </row>
     <row r="117" spans="1:19">
       <c r="A117" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B117" t="s">
         <v>20</v>
@@ -5980,28 +5990,28 @@
         <v>22</v>
       </c>
       <c r="D117" s="18" t="s">
+        <v>446</v>
+      </c>
+      <c r="I117" s="8" t="s">
         <v>447</v>
-      </c>
-      <c r="I117" s="8" t="s">
-        <v>448</v>
       </c>
       <c r="K117" s="18">
         <v>24</v>
       </c>
       <c r="L117" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M117" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R117" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="S117" s="19"/>
     </row>
     <row r="118" spans="1:19">
       <c r="A118" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B118" t="s">
         <v>20</v>
@@ -6010,28 +6020,28 @@
         <v>22</v>
       </c>
       <c r="D118" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="I118" s="8" t="s">
         <v>337</v>
-      </c>
-      <c r="I118" s="8" t="s">
-        <v>338</v>
       </c>
       <c r="K118" s="18">
         <v>33</v>
       </c>
       <c r="L118" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M118" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R118" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="S118" s="19"/>
     </row>
     <row r="119" spans="1:19">
       <c r="A119" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B119" t="s">
         <v>20</v>
@@ -6040,28 +6050,28 @@
         <v>22</v>
       </c>
       <c r="D119" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="I119" s="8" t="s">
         <v>341</v>
-      </c>
-      <c r="I119" s="8" t="s">
-        <v>342</v>
       </c>
       <c r="K119" s="18">
         <v>42</v>
       </c>
       <c r="L119" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M119" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R119" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="S119" s="19"/>
     </row>
     <row r="120" spans="1:19">
       <c r="A120" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B120" t="s">
         <v>20</v>
@@ -6070,28 +6080,28 @@
         <v>22</v>
       </c>
       <c r="D120" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="I120" s="8" t="s">
         <v>345</v>
-      </c>
-      <c r="I120" s="8" t="s">
-        <v>346</v>
       </c>
       <c r="K120" s="18">
         <v>37</v>
       </c>
       <c r="L120" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M120" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R120" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="S120" s="19"/>
     </row>
     <row r="121" spans="1:19">
       <c r="A121" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B121" t="s">
         <v>20</v>
@@ -6100,28 +6110,28 @@
         <v>22</v>
       </c>
       <c r="D121" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="I121" s="8" t="s">
         <v>349</v>
-      </c>
-      <c r="I121" s="8" t="s">
-        <v>350</v>
       </c>
       <c r="K121" s="18">
         <v>33</v>
       </c>
       <c r="L121" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="M121" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="M121" s="18" t="s">
-        <v>161</v>
-      </c>
       <c r="R121" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="S121" s="19"/>
     </row>
     <row r="122" spans="1:19">
       <c r="A122" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B122" t="s">
         <v>20</v>
@@ -6131,25 +6141,25 @@
       </c>
       <c r="D122" s="18"/>
       <c r="I122" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="K122" s="18">
         <v>31</v>
       </c>
       <c r="L122" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M122" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="R122" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="S122" s="19"/>
     </row>
     <row r="123" spans="1:19">
       <c r="A123" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B123" t="s">
         <v>20</v>
@@ -6158,28 +6168,28 @@
         <v>22</v>
       </c>
       <c r="D123" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="I123" s="8" t="s">
         <v>355</v>
-      </c>
-      <c r="I123" s="8" t="s">
-        <v>356</v>
       </c>
       <c r="K123" s="18">
         <v>34</v>
       </c>
       <c r="L123" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M123" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R123" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="S123" s="19"/>
     </row>
     <row r="124" spans="1:19">
       <c r="A124" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B124" t="s">
         <v>20</v>
@@ -6189,25 +6199,25 @@
       </c>
       <c r="D124" s="18"/>
       <c r="I124" s="8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K124" s="18">
         <v>36</v>
       </c>
       <c r="L124" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M124" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="R124" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="S124" s="19"/>
     </row>
     <row r="125" spans="1:19">
       <c r="A125" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B125" t="s">
         <v>20</v>
@@ -6217,25 +6227,25 @@
       </c>
       <c r="D125" s="8"/>
       <c r="I125" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K125" s="18">
         <v>45</v>
       </c>
       <c r="L125" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M125" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R125" s="15" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="S125" s="19"/>
     </row>
     <row r="126" spans="1:19">
       <c r="A126" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B126" t="s">
         <v>20</v>
@@ -6244,28 +6254,28 @@
         <v>22</v>
       </c>
       <c r="D126" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="I126" s="8" t="s">
         <v>365</v>
-      </c>
-      <c r="I126" s="8" t="s">
-        <v>366</v>
       </c>
       <c r="K126" s="18">
         <v>42</v>
       </c>
       <c r="L126" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M126" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="R126" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="S126" s="19"/>
     </row>
     <row r="127" spans="1:19">
       <c r="A127" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B127" t="s">
         <v>20</v>
@@ -6275,25 +6285,25 @@
       </c>
       <c r="D127" s="18"/>
       <c r="I127" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K127" s="18">
         <v>40</v>
       </c>
       <c r="L127" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M127" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R127" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="S127" s="19"/>
     </row>
     <row r="128" spans="1:19">
       <c r="A128" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B128" t="s">
         <v>20</v>
@@ -6302,28 +6312,28 @@
         <v>22</v>
       </c>
       <c r="D128" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="I128" s="8" t="s">
         <v>372</v>
-      </c>
-      <c r="I128" s="8" t="s">
-        <v>373</v>
       </c>
       <c r="K128" s="18">
         <v>30</v>
       </c>
       <c r="L128" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="M128" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="R128" t="s">
         <v>161</v>
-      </c>
-      <c r="M128" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="R128" t="s">
-        <v>162</v>
       </c>
       <c r="S128" s="19"/>
     </row>
     <row r="129" spans="1:19">
       <c r="A129" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B129" t="s">
         <v>20</v>
@@ -6332,28 +6342,28 @@
         <v>22</v>
       </c>
       <c r="D129" s="18" t="s">
+        <v>374</v>
+      </c>
+      <c r="I129" s="8" t="s">
         <v>375</v>
-      </c>
-      <c r="I129" s="8" t="s">
-        <v>376</v>
       </c>
       <c r="K129" s="18">
         <v>49</v>
       </c>
       <c r="L129" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="M129" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="R129" t="s">
         <v>161</v>
-      </c>
-      <c r="M129" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="R129" t="s">
-        <v>162</v>
       </c>
       <c r="S129" s="19"/>
     </row>
     <row r="130" spans="1:19">
       <c r="A130" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B130" t="s">
         <v>20</v>
@@ -6362,28 +6372,28 @@
         <v>22</v>
       </c>
       <c r="D130" s="18" t="s">
+        <v>377</v>
+      </c>
+      <c r="I130" s="8" t="s">
         <v>378</v>
-      </c>
-      <c r="I130" s="8" t="s">
-        <v>379</v>
       </c>
       <c r="K130" s="18">
         <v>38</v>
       </c>
       <c r="L130" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M130" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R130" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="S130" s="19"/>
     </row>
     <row r="131" spans="1:19">
       <c r="A131" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B131" t="s">
         <v>20</v>
@@ -6392,28 +6402,28 @@
         <v>22</v>
       </c>
       <c r="D131" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="I131" s="8" t="s">
         <v>382</v>
-      </c>
-      <c r="I131" s="8" t="s">
-        <v>383</v>
       </c>
       <c r="K131" s="18">
         <v>35</v>
       </c>
       <c r="L131" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M131" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="R131" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="S131" s="19"/>
     </row>
     <row r="132" spans="1:19">
       <c r="A132" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B132" t="s">
         <v>20</v>
@@ -6423,25 +6433,25 @@
       </c>
       <c r="D132" s="18"/>
       <c r="I132" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K132" s="18">
         <v>35</v>
       </c>
       <c r="L132" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M132" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R132" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S132" s="19"/>
     </row>
     <row r="133" spans="1:19">
       <c r="A133" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B133" t="s">
         <v>20</v>
@@ -6450,28 +6460,28 @@
         <v>22</v>
       </c>
       <c r="D133" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="I133" s="8" t="s">
         <v>389</v>
-      </c>
-      <c r="I133" s="8" t="s">
-        <v>390</v>
       </c>
       <c r="K133" s="18">
         <v>37</v>
       </c>
       <c r="L133" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M133" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="R133" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="S133" s="19"/>
     </row>
     <row r="134" spans="1:19">
       <c r="A134" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B134" t="s">
         <v>24</v>
@@ -6480,35 +6490,35 @@
         <v>21</v>
       </c>
       <c r="D134" s="18" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H134" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I134" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="R134" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="S134" s="19"/>
     </row>
     <row r="135" spans="1:19">
       <c r="D135" s="18"/>
       <c r="H135" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I135" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="R135" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="S135" s="19"/>
     </row>
     <row r="136" spans="1:19">
       <c r="A136" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B136" t="s">
         <v>24</v>
@@ -6518,32 +6528,32 @@
       </c>
       <c r="D136" s="18"/>
       <c r="H136" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I136" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="R136" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="S136" s="19"/>
     </row>
     <row r="137" spans="1:19">
       <c r="D137" s="18"/>
       <c r="H137" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I137" s="8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="R137" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="S137" s="19"/>
     </row>
     <row r="138" spans="1:19">
       <c r="A138" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B138" t="s">
         <v>24</v>
@@ -6552,21 +6562,21 @@
         <v>25</v>
       </c>
       <c r="D138" s="18" t="s">
+        <v>397</v>
+      </c>
+      <c r="I138" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="R138" t="s">
         <v>398</v>
       </c>
-      <c r="I138" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="R138" t="s">
-        <v>399</v>
-      </c>
       <c r="S138" s="19" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="139" spans="1:19">
       <c r="A139" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B139" t="s">
         <v>24</v>
@@ -6575,21 +6585,21 @@
         <v>25</v>
       </c>
       <c r="D139" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="I139" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="R139" t="s">
         <v>401</v>
       </c>
-      <c r="I139" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="R139" t="s">
-        <v>402</v>
-      </c>
       <c r="S139" s="19" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="140" spans="1:19">
       <c r="A140" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B140" t="s">
         <v>24</v>
@@ -6598,21 +6608,21 @@
         <v>25</v>
       </c>
       <c r="D140" s="18" t="s">
+        <v>403</v>
+      </c>
+      <c r="I140" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="R140" t="s">
         <v>404</v>
       </c>
-      <c r="I140" s="8" t="s">
-        <v>442</v>
-      </c>
-      <c r="R140" t="s">
-        <v>405</v>
-      </c>
       <c r="S140" s="19" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="141" spans="1:19">
       <c r="A141" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B141" t="s">
         <v>24</v>
@@ -6621,16 +6631,16 @@
         <v>25</v>
       </c>
       <c r="D141" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="I141" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="R141" t="s">
         <v>407</v>
       </c>
-      <c r="I141" s="8" t="s">
-        <v>443</v>
-      </c>
-      <c r="R141" t="s">
-        <v>408</v>
-      </c>
       <c r="S141" s="19" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="142" spans="1:19">

</xml_diff>